<commit_message>
int letter and  int packages
</commit_message>
<xml_diff>
--- a/calc/files/packages_int.xlsx
+++ b/calc/files/packages_int.xlsx
@@ -36,7 +36,7 @@
         <rFont val="Microsoft Sans Serif"/>
         <sz val="9.5"/>
       </rPr>
-      <t>23 сентября  2025 № 869</t>
+      <t>от 05.11.2025 № 1018</t>
     </r>
   </si>
   <si>
@@ -58,7 +58,7 @@
         <color rgb="FF0000" tint="0"/>
         <sz val="9.5"/>
       </rPr>
-      <t>в действии с 01.10.2025</t>
+      <t>в действии с 10.11.2025</t>
     </r>
   </si>
   <si>
@@ -121,7 +121,7 @@
         <rFont val="Microsoft Sans Serif"/>
         <sz val="9.5"/>
       </rPr>
-      <t>за отправлени е</t>
+      <t>за отправление</t>
     </r>
   </si>
   <si>
@@ -131,15 +131,6 @@
         <sz val="9.5"/>
       </rPr>
       <t>за кг</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Microsoft Sans Serif"/>
-        <sz val="9.5"/>
-      </rPr>
-      <t>за отправление</t>
     </r>
   </si>
   <si>
@@ -2196,7 +2187,7 @@
         <rFont val="Microsoft Sans Serif"/>
         <sz val="9.5"/>
       </rPr>
-      <t>Тарификация за массу регистируемого мелкого пакета осуществляется с точностью до десятков граммов. Любое количество граммов округляется до десятков граммов в большую сторону</t>
+      <t>Международные мелкие пакеты принимаются только с товарным вложением</t>
     </r>
   </si>
   <si>
@@ -2241,10 +2232,10 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <b val="true"/>
-        <sz val="9.5"/>
-      </rPr>
-      <t>Заказные мелкие пакеты</t>
+        <b val="false"/>
+        <sz val="9.5"/>
+      </rPr>
+      <t>Тарификация за массу мелкого пакета отслеживаемого осуществляется с точностью до сотен граммов. Любое количество граммов округляется до сотен в большую сторону</t>
     </r>
   </si>
   <si>
@@ -2252,43 +2243,6 @@
       <rPr>
         <rFont val="Arial"/>
         <b val="true"/>
-        <sz val="8.5"/>
-      </rPr>
-      <t>неприоритетная*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Microsoft Sans Serif"/>
-        <sz val="9.5"/>
-      </rPr>
-      <t>Плата за массу взимается согласно тарифам ст.1  в зависимости от способа пересылки (неприоритетная или приоритетная). Дополнительно взимается плата за заказ и дополнительную обработку (поз.229).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Microsoft Sans Serif"/>
-        <sz val="9.5"/>
-      </rPr>
-      <t>Плата за заказ (независимо от массы) и дополнительную обработку, за одно отправление</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Microsoft Sans Serif"/>
-        <sz val="9.5"/>
-      </rPr>
-      <t>*прием и пересылка  неприоритетных регистрируемых мелких пакетов осуществляется только в Российскую Федерацию</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b val="true"/>
         <sz val="9.5"/>
       </rPr>
       <t>Примечание:</t>
@@ -2301,11 +2255,7 @@
         <color rgb="000000" tint="0"/>
         <sz val="9.5"/>
       </rPr>
-      <t>Сверх размера оплаты за услуги, оказываемые юридическим лицам и индивидуальным, предпринимателям взимается налог на добавленную стоимость в соответствии с</t>
-    </r>
-    <r>
-      <t xml:space="preserve">
-</t>
+      <t xml:space="preserve">Сверх размера оплаты за услуги, оказываемые юридическим лицам и индивидуальным, предпринимателям взимается налог на добавленную стоимость в соответствии с </t>
     </r>
     <r>
       <rPr>
@@ -2322,11 +2272,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a15="http://schemas.microsoft.com/office/drawing/2012/main" xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:co="http://ncloudtech.com" xmlns:co-ooxml="http://ncloudtech.com/ooxml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:x="urn:schemas-microsoft-com:office:excel" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" mc:Ignorable="co co-ooxml w14 x14 w15">
   <numFmts>
-    <numFmt co:extendedFormatCode="0" formatCode="0" numFmtId="1001"/>
+    <numFmt co:extendedFormatCode="General" formatCode="General" numFmtId="1002"/>
+    <numFmt co:extendedFormatCode="0.00" formatCode="0.00" numFmtId="1005"/>
+    <numFmt co:extendedFormatCode="General" formatCode="General" numFmtId="1001"/>
     <numFmt co:extendedFormatCode="General" formatCode="General" numFmtId="1000"/>
-    <numFmt co:extendedFormatCode="0.00" formatCode="0.00" numFmtId="1002"/>
+    <numFmt co:extendedFormatCode="General" formatCode="General" numFmtId="1003"/>
+    <numFmt co:extendedFormatCode="0" formatCode="0" numFmtId="1004"/>
+    <numFmt co:extendedFormatCode="General" formatCode="General" numFmtId="1006"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <name val="Calibri"/>
       <sz val="11"/>
@@ -2383,16 +2337,31 @@
       <b val="true"/>
       <sz val="8.5"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <b val="false"/>
+      <sz val="9.5"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F2F2F2" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.25"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="63">
+  <borders count="54">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -2400,47 +2369,70 @@
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
+    <border diagonalDown="true" diagonalUp="true">
+      <left style="none">
+        <color rgb="000000" tint="0"/>
+      </left>
+      <right style="none">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="none">
+        <color rgb="000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000" tint="0"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="000000" tint="0"/>
+      </diagonal>
+    </border>
     <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
+      <top style="none">
+        <color rgb="000000" tint="0"/>
+      </top>
       <bottom style="thin">
         <color rgb="000000" tint="0"/>
       </bottom>
     </border>
     <border>
-      <top style="none"/>
+      <top style="none">
+        <color rgb="000000" tint="0"/>
+      </top>
       <bottom style="thin">
         <color rgb="000000" tint="0"/>
       </bottom>
     </border>
     <border>
-      <top style="none"/>
+      <top style="none">
+        <color rgb="000000" tint="0"/>
+      </top>
       <bottom style="thin">
         <color rgb="000000" tint="0"/>
       </bottom>
     </border>
     <border>
-      <top style="none"/>
+      <top style="none">
+        <color rgb="000000" tint="0"/>
+      </top>
       <bottom style="thin">
         <color rgb="000000" tint="0"/>
       </bottom>
     </border>
     <border>
-      <top style="none"/>
+      <top style="none">
+        <color rgb="000000" tint="0"/>
+      </top>
       <bottom style="thin">
         <color rgb="000000" tint="0"/>
       </bottom>
     </border>
     <border>
-      <top style="none"/>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="none"/>
-      <top style="none"/>
+      <right style="none">
+        <color rgb="000000" tint="0"/>
+      </right>
+      <top style="none">
+        <color rgb="000000" tint="0"/>
+      </top>
       <bottom style="thin">
         <color rgb="000000" tint="0"/>
       </bottom>
@@ -2663,93 +2655,6 @@
       </bottom>
     </border>
     <border>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="000000" tint="0"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="000000" tint="0"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="000000" tint="0"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="000000" tint="0"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000" tint="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="000000" tint="0"/>
-      </right>
       <top style="thin">
         <color rgb="000000" tint="0"/>
       </top>
@@ -2966,7 +2871,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="80">
     <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="1" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2976,34 +2881,34 @@
     <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="right" indent="2" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="2" numFmtId="1001" quotePrefix="false">
       <alignment horizontal="right" indent="1" vertical="top" wrapText="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="3" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" indent="7" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="1" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="4" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="right" indent="2" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="1" fillId="0" fontId="5" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="1" fillId="0" fontId="5" numFmtId="1002" quotePrefix="false">
       <alignment horizontal="right" indent="2" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="5" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="5" numFmtId="1002" quotePrefix="false">
       <alignment horizontal="right" indent="2" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="5" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="5" numFmtId="1002" quotePrefix="false">
       <alignment horizontal="right" indent="2" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="4" fillId="0" fontId="5" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="4" fillId="0" fontId="5" numFmtId="1002" quotePrefix="false">
       <alignment horizontal="right" indent="2" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="5" fillId="0" fontId="5" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="5" fillId="0" fontId="5" numFmtId="1002" quotePrefix="false">
       <alignment horizontal="right" indent="2" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="6" fillId="0" fontId="5" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="6" fillId="0" fontId="5" numFmtId="1002" quotePrefix="false">
       <alignment horizontal="right" indent="2" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="7" fillId="0" fontId="5" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="7" fillId="0" fontId="5" numFmtId="1002" quotePrefix="false">
       <alignment horizontal="right" indent="2" vertical="top" wrapText="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
@@ -3051,41 +2956,44 @@
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="19" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" indent="4" vertical="center" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="2" numFmtId="1003" quotePrefix="false">
       <alignment horizontal="center" vertical="top" wrapText="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="1" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="6" numFmtId="1001" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="6" numFmtId="1004" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="7" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="8" numFmtId="1001" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="8" numFmtId="1004" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="1" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="bottom" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="8" numFmtId="1002" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="8" numFmtId="1005" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="8" numFmtId="1001" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="8" numFmtId="1004" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="8" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="8" numFmtId="1002" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="8" numFmtId="1005" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="8" fillId="2" fontId="8" numFmtId="1005" quotePrefix="false">
+      <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="9" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
@@ -3162,73 +3070,46 @@
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="40" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="41" fillId="0" fontId="8" numFmtId="1002" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="41" fillId="0" fontId="8" numFmtId="1005" quotePrefix="false">
       <alignment horizontal="center" shrinkToFit="true" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="10" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" indent="2" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="42" fillId="0" fontId="10" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" indent="2" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="43" fillId="0" fontId="10" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" indent="5" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="44" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="8" fillId="3" fontId="11" numFmtId="1006" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="45" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="42" fillId="3" fontId="11" numFmtId="1006" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="46" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="43" fillId="3" fontId="11" numFmtId="1006" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="47" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="44" fillId="3" fontId="11" numFmtId="1006" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="48" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="45" fillId="3" fontId="11" numFmtId="1006" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="49" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="46" fillId="0" fontId="7" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="50" fillId="0" fontId="8" numFmtId="1002" quotePrefix="false">
-      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="51" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="47" fillId="0" fontId="7" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="52" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="48" fillId="0" fontId="7" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="53" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="49" fillId="0" fontId="7" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="54" fillId="0" fontId="2" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="50" fillId="0" fontId="8" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="55" fillId="0" fontId="7" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="51" fillId="0" fontId="8" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="56" fillId="0" fontId="7" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="52" fillId="0" fontId="8" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="57" fillId="0" fontId="7" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="58" fillId="0" fontId="7" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="59" fillId="0" fontId="8" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="60" fillId="0" fontId="8" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="61" fillId="0" fontId="8" numFmtId="1000" quotePrefix="false">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="62" fillId="0" fontId="8" numFmtId="1000" quotePrefix="false">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" borderId="53" fillId="0" fontId="8" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -3449,7 +3330,7 @@
   <sheetPr>
     <outlinePr summaryBelow="true" summaryRight="true"/>
   </sheetPr>
-  <dimension ref="A1:G244"/>
+  <dimension ref="A1:G245"/>
   <sheetViews>
     <sheetView showZeros="true" workbookViewId="0"/>
   </sheetViews>
@@ -3460,7 +3341,7 @@
     <col customWidth="true" max="3" min="3" outlineLevel="0" width="38.2360203182117"/>
     <col customWidth="true" max="4" min="4" outlineLevel="0" width="11.6284806153318"/>
     <col customWidth="true" max="5" min="5" outlineLevel="0" width="11.8255727501701"/>
-    <col customWidth="true" max="6" min="6" outlineLevel="0" width="14.584873464542"/>
+    <col customWidth="true" max="6" min="6" outlineLevel="0" width="12.4266986864415"/>
     <col customWidth="true" max="7" min="7" outlineLevel="0" width="13.0081309725178"/>
   </cols>
   <sheetData>
@@ -3568,33 +3449,33 @@
       <c r="E9" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="30" t="s">
-        <v>13</v>
+      <c r="F9" s="28" t="s">
+        <v>11</v>
       </c>
       <c r="G9" s="29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row customHeight="true" ht="26" outlineLevel="0" r="10">
-      <c r="A10" s="31" t="n"/>
-      <c r="B10" s="32" t="n">
+    <row customHeight="true" ht="15.25" outlineLevel="0" r="10">
+      <c r="A10" s="30" t="n"/>
+      <c r="B10" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="30" t="n"/>
+      <c r="E10" s="30" t="n"/>
+      <c r="F10" s="30" t="n"/>
+      <c r="G10" s="30" t="n"/>
+    </row>
+    <row customHeight="true" ht="13.5" outlineLevel="0" r="11">
+      <c r="A11" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" s="34" t="n"/>
+      <c r="C11" s="35" t="s">
         <v>14</v>
-      </c>
-      <c r="D10" s="31" t="n"/>
-      <c r="E10" s="31" t="n"/>
-      <c r="F10" s="31" t="n"/>
-      <c r="G10" s="31" t="n"/>
-    </row>
-    <row customHeight="true" ht="13.5" outlineLevel="0" r="11">
-      <c r="A11" s="34" t="n">
-        <v>1</v>
-      </c>
-      <c r="B11" s="35" t="n"/>
-      <c r="C11" s="30" t="s">
-        <v>15</v>
       </c>
       <c r="D11" s="36" t="n">
         <v>6.25</v>
@@ -3610,12 +3491,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="12">
-      <c r="A12" s="34" t="n">
+      <c r="A12" s="33" t="n">
         <v>2</v>
       </c>
-      <c r="B12" s="35" t="n"/>
-      <c r="C12" s="30" t="s">
-        <v>16</v>
+      <c r="B12" s="34" t="n"/>
+      <c r="C12" s="35" t="s">
+        <v>15</v>
       </c>
       <c r="D12" s="36" t="n">
         <v>6.5</v>
@@ -3631,12 +3512,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="13">
-      <c r="A13" s="34" t="n">
+      <c r="A13" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="B13" s="35" t="n"/>
-      <c r="C13" s="30" t="s">
-        <v>17</v>
+      <c r="B13" s="34" t="n"/>
+      <c r="C13" s="35" t="s">
+        <v>16</v>
       </c>
       <c r="D13" s="36" t="n">
         <v>4.5</v>
@@ -3652,12 +3533,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="14">
-      <c r="A14" s="34" t="n">
+      <c r="A14" s="33" t="n">
         <v>4</v>
       </c>
-      <c r="B14" s="35" t="n"/>
-      <c r="C14" s="30" t="s">
-        <v>18</v>
+      <c r="B14" s="34" t="n"/>
+      <c r="C14" s="35" t="s">
+        <v>17</v>
       </c>
       <c r="D14" s="36" t="n">
         <v>4.75</v>
@@ -3673,12 +3554,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="15">
-      <c r="A15" s="34" t="n">
+      <c r="A15" s="33" t="n">
         <v>5</v>
       </c>
-      <c r="B15" s="35" t="n"/>
-      <c r="C15" s="30" t="s">
-        <v>19</v>
+      <c r="B15" s="34" t="n"/>
+      <c r="C15" s="35" t="s">
+        <v>18</v>
       </c>
       <c r="D15" s="36" t="n">
         <v>4.5</v>
@@ -3694,12 +3575,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="16">
-      <c r="A16" s="34" t="n">
+      <c r="A16" s="33" t="n">
         <v>6</v>
       </c>
-      <c r="B16" s="35" t="n"/>
-      <c r="C16" s="30" t="s">
-        <v>20</v>
+      <c r="B16" s="34" t="n"/>
+      <c r="C16" s="35" t="s">
+        <v>19</v>
       </c>
       <c r="D16" s="36" t="n">
         <v>4.5</v>
@@ -3715,12 +3596,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="17">
-      <c r="A17" s="34" t="n">
+      <c r="A17" s="33" t="n">
         <v>7</v>
       </c>
-      <c r="B17" s="35" t="n"/>
-      <c r="C17" s="30" t="s">
-        <v>21</v>
+      <c r="B17" s="34" t="n"/>
+      <c r="C17" s="35" t="s">
+        <v>20</v>
       </c>
       <c r="D17" s="36" t="n">
         <v>5.5</v>
@@ -3736,12 +3617,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="18">
-      <c r="A18" s="34" t="n">
+      <c r="A18" s="33" t="n">
         <v>8</v>
       </c>
-      <c r="B18" s="35" t="n"/>
-      <c r="C18" s="30" t="s">
-        <v>22</v>
+      <c r="B18" s="34" t="n"/>
+      <c r="C18" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="D18" s="36" t="n">
         <v>4.5</v>
@@ -3757,12 +3638,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="19">
-      <c r="A19" s="34" t="n">
+      <c r="A19" s="33" t="n">
         <v>9</v>
       </c>
-      <c r="B19" s="35" t="n"/>
-      <c r="C19" s="30" t="s">
-        <v>23</v>
+      <c r="B19" s="34" t="n"/>
+      <c r="C19" s="35" t="s">
+        <v>22</v>
       </c>
       <c r="D19" s="36" t="n">
         <v>4.5</v>
@@ -3778,12 +3659,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="20">
-      <c r="A20" s="34" t="n">
+      <c r="A20" s="33" t="n">
         <v>10</v>
       </c>
-      <c r="B20" s="35" t="n"/>
-      <c r="C20" s="30" t="s">
-        <v>24</v>
+      <c r="B20" s="34" t="n"/>
+      <c r="C20" s="35" t="s">
+        <v>23</v>
       </c>
       <c r="D20" s="36" t="n">
         <v>6.75</v>
@@ -3799,12 +3680,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="21">
-      <c r="A21" s="34" t="n">
+      <c r="A21" s="33" t="n">
         <v>11</v>
       </c>
-      <c r="B21" s="35" t="n"/>
-      <c r="C21" s="30" t="s">
-        <v>25</v>
+      <c r="B21" s="34" t="n"/>
+      <c r="C21" s="35" t="s">
+        <v>24</v>
       </c>
       <c r="D21" s="36" t="n">
         <v>4.5</v>
@@ -3820,12 +3701,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="22">
-      <c r="A22" s="34" t="n">
+      <c r="A22" s="33" t="n">
         <v>12</v>
       </c>
-      <c r="B22" s="35" t="n"/>
-      <c r="C22" s="30" t="s">
-        <v>26</v>
+      <c r="B22" s="34" t="n"/>
+      <c r="C22" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="D22" s="36" t="n">
         <v>4.5</v>
@@ -3841,12 +3722,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="23">
-      <c r="A23" s="34" t="n">
+      <c r="A23" s="33" t="n">
         <v>13</v>
       </c>
-      <c r="B23" s="35" t="n"/>
-      <c r="C23" s="30" t="s">
-        <v>27</v>
+      <c r="B23" s="34" t="n"/>
+      <c r="C23" s="35" t="s">
+        <v>26</v>
       </c>
       <c r="D23" s="36" t="n">
         <v>4.5</v>
@@ -3862,12 +3743,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="24">
-      <c r="A24" s="34" t="n">
+      <c r="A24" s="33" t="n">
         <v>14</v>
       </c>
-      <c r="B24" s="35" t="n"/>
-      <c r="C24" s="30" t="s">
-        <v>28</v>
+      <c r="B24" s="34" t="n"/>
+      <c r="C24" s="35" t="s">
+        <v>27</v>
       </c>
       <c r="D24" s="36" t="n">
         <v>4.5</v>
@@ -3883,12 +3764,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="25">
-      <c r="A25" s="34" t="n">
+      <c r="A25" s="33" t="n">
         <v>15</v>
       </c>
-      <c r="B25" s="35" t="n"/>
-      <c r="C25" s="30" t="s">
-        <v>29</v>
+      <c r="B25" s="34" t="n"/>
+      <c r="C25" s="35" t="s">
+        <v>28</v>
       </c>
       <c r="D25" s="36" t="n">
         <v>4.5</v>
@@ -3904,12 +3785,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="26">
-      <c r="A26" s="34" t="n">
+      <c r="A26" s="33" t="n">
         <v>16</v>
       </c>
-      <c r="B26" s="35" t="n"/>
-      <c r="C26" s="30" t="s">
-        <v>30</v>
+      <c r="B26" s="34" t="n"/>
+      <c r="C26" s="35" t="s">
+        <v>29</v>
       </c>
       <c r="D26" s="36" t="n">
         <v>4.5</v>
@@ -3925,12 +3806,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="27">
-      <c r="A27" s="34" t="n">
+      <c r="A27" s="33" t="n">
         <v>17</v>
       </c>
-      <c r="B27" s="35" t="n"/>
-      <c r="C27" s="30" t="s">
-        <v>31</v>
+      <c r="B27" s="34" t="n"/>
+      <c r="C27" s="35" t="s">
+        <v>30</v>
       </c>
       <c r="D27" s="36" t="n">
         <v>4.5</v>
@@ -3946,12 +3827,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="28">
-      <c r="A28" s="34" t="n">
+      <c r="A28" s="33" t="n">
         <v>18</v>
       </c>
-      <c r="B28" s="35" t="n"/>
-      <c r="C28" s="30" t="s">
-        <v>32</v>
+      <c r="B28" s="34" t="n"/>
+      <c r="C28" s="35" t="s">
+        <v>31</v>
       </c>
       <c r="D28" s="36" t="n">
         <v>4.5</v>
@@ -3967,12 +3848,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="29">
-      <c r="A29" s="34" t="n">
+      <c r="A29" s="33" t="n">
         <v>19</v>
       </c>
-      <c r="B29" s="35" t="n"/>
-      <c r="C29" s="30" t="s">
-        <v>33</v>
+      <c r="B29" s="34" t="n"/>
+      <c r="C29" s="35" t="s">
+        <v>32</v>
       </c>
       <c r="D29" s="36" t="n">
         <v>7</v>
@@ -3988,12 +3869,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="30">
-      <c r="A30" s="34" t="n">
+      <c r="A30" s="33" t="n">
         <v>20</v>
       </c>
-      <c r="B30" s="35" t="n"/>
-      <c r="C30" s="30" t="s">
-        <v>34</v>
+      <c r="B30" s="34" t="n"/>
+      <c r="C30" s="35" t="s">
+        <v>33</v>
       </c>
       <c r="D30" s="36" t="n">
         <v>4.5</v>
@@ -4009,12 +3890,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="31">
-      <c r="A31" s="34" t="n">
+      <c r="A31" s="33" t="n">
         <v>21</v>
       </c>
-      <c r="B31" s="35" t="n"/>
-      <c r="C31" s="30" t="s">
-        <v>35</v>
+      <c r="B31" s="34" t="n"/>
+      <c r="C31" s="35" t="s">
+        <v>34</v>
       </c>
       <c r="D31" s="36" t="n">
         <v>4.5</v>
@@ -4030,12 +3911,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="32">
-      <c r="A32" s="34" t="n">
+      <c r="A32" s="33" t="n">
         <v>22</v>
       </c>
-      <c r="B32" s="35" t="n"/>
-      <c r="C32" s="30" t="s">
-        <v>36</v>
+      <c r="B32" s="34" t="n"/>
+      <c r="C32" s="35" t="s">
+        <v>35</v>
       </c>
       <c r="D32" s="36" t="n">
         <v>7</v>
@@ -4051,12 +3932,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="33">
-      <c r="A33" s="34" t="n">
+      <c r="A33" s="33" t="n">
         <v>23</v>
       </c>
-      <c r="B33" s="35" t="n"/>
-      <c r="C33" s="30" t="s">
-        <v>37</v>
+      <c r="B33" s="34" t="n"/>
+      <c r="C33" s="35" t="s">
+        <v>36</v>
       </c>
       <c r="D33" s="36" t="n">
         <v>4.5</v>
@@ -4072,12 +3953,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="34">
-      <c r="A34" s="34" t="n">
+      <c r="A34" s="33" t="n">
         <v>24</v>
       </c>
-      <c r="B34" s="35" t="n"/>
-      <c r="C34" s="30" t="s">
-        <v>38</v>
+      <c r="B34" s="34" t="n"/>
+      <c r="C34" s="35" t="s">
+        <v>37</v>
       </c>
       <c r="D34" s="36" t="n">
         <v>6.75</v>
@@ -4093,12 +3974,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="35">
-      <c r="A35" s="34" t="n">
+      <c r="A35" s="33" t="n">
         <v>25</v>
       </c>
-      <c r="B35" s="35" t="n"/>
-      <c r="C35" s="30" t="s">
-        <v>39</v>
+      <c r="B35" s="34" t="n"/>
+      <c r="C35" s="35" t="s">
+        <v>38</v>
       </c>
       <c r="D35" s="36" t="n">
         <v>6.25</v>
@@ -4114,12 +3995,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="36">
-      <c r="A36" s="34" t="n">
+      <c r="A36" s="33" t="n">
         <v>26</v>
       </c>
-      <c r="B36" s="35" t="n"/>
-      <c r="C36" s="30" t="s">
-        <v>40</v>
+      <c r="B36" s="34" t="n"/>
+      <c r="C36" s="35" t="s">
+        <v>39</v>
       </c>
       <c r="D36" s="36" t="n">
         <v>4.75</v>
@@ -4135,12 +4016,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="37">
-      <c r="A37" s="34" t="n">
+      <c r="A37" s="33" t="n">
         <v>27</v>
       </c>
-      <c r="B37" s="35" t="n"/>
-      <c r="C37" s="30" t="s">
-        <v>41</v>
+      <c r="B37" s="34" t="n"/>
+      <c r="C37" s="35" t="s">
+        <v>40</v>
       </c>
       <c r="D37" s="36" t="n">
         <v>4.5</v>
@@ -4156,12 +4037,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="38">
-      <c r="A38" s="34" t="n">
+      <c r="A38" s="33" t="n">
         <v>28</v>
       </c>
-      <c r="B38" s="35" t="n"/>
-      <c r="C38" s="30" t="s">
-        <v>42</v>
+      <c r="B38" s="34" t="n"/>
+      <c r="C38" s="35" t="s">
+        <v>41</v>
       </c>
       <c r="D38" s="36" t="n">
         <v>4.5</v>
@@ -4177,12 +4058,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="39">
-      <c r="A39" s="34" t="n">
+      <c r="A39" s="33" t="n">
         <v>29</v>
       </c>
-      <c r="B39" s="35" t="n"/>
-      <c r="C39" s="30" t="s">
-        <v>43</v>
+      <c r="B39" s="34" t="n"/>
+      <c r="C39" s="35" t="s">
+        <v>42</v>
       </c>
       <c r="D39" s="36" t="n">
         <v>4.5</v>
@@ -4198,12 +4079,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="40">
-      <c r="A40" s="34" t="n">
+      <c r="A40" s="33" t="n">
         <v>30</v>
       </c>
-      <c r="B40" s="35" t="n"/>
-      <c r="C40" s="30" t="s">
-        <v>44</v>
+      <c r="B40" s="34" t="n"/>
+      <c r="C40" s="35" t="s">
+        <v>43</v>
       </c>
       <c r="D40" s="36" t="n">
         <v>4.5</v>
@@ -4219,12 +4100,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="41">
-      <c r="A41" s="34" t="n">
+      <c r="A41" s="33" t="n">
         <v>31</v>
       </c>
-      <c r="B41" s="35" t="n"/>
-      <c r="C41" s="30" t="s">
-        <v>45</v>
+      <c r="B41" s="34" t="n"/>
+      <c r="C41" s="35" t="s">
+        <v>44</v>
       </c>
       <c r="D41" s="36" t="n">
         <v>4.5</v>
@@ -4240,12 +4121,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="42">
-      <c r="A42" s="34" t="n">
+      <c r="A42" s="33" t="n">
         <v>32</v>
       </c>
-      <c r="B42" s="35" t="n"/>
-      <c r="C42" s="30" t="s">
-        <v>46</v>
+      <c r="B42" s="34" t="n"/>
+      <c r="C42" s="35" t="s">
+        <v>45</v>
       </c>
       <c r="D42" s="36" t="n">
         <v>4.5</v>
@@ -4261,12 +4142,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="43">
-      <c r="A43" s="34" t="n">
+      <c r="A43" s="33" t="n">
         <v>33</v>
       </c>
-      <c r="B43" s="35" t="n"/>
-      <c r="C43" s="30" t="s">
-        <v>47</v>
+      <c r="B43" s="34" t="n"/>
+      <c r="C43" s="35" t="s">
+        <v>46</v>
       </c>
       <c r="D43" s="36" t="n">
         <v>7</v>
@@ -4285,9 +4166,9 @@
       <c r="A44" s="37" t="n">
         <v>34</v>
       </c>
-      <c r="B44" s="31" t="n"/>
+      <c r="B44" s="30" t="n"/>
       <c r="C44" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D44" s="39" t="n">
         <v>7</v>
@@ -4303,12 +4184,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="45">
-      <c r="A45" s="34" t="n">
+      <c r="A45" s="33" t="n">
         <v>35</v>
       </c>
-      <c r="B45" s="35" t="n"/>
-      <c r="C45" s="30" t="s">
-        <v>49</v>
+      <c r="B45" s="34" t="n"/>
+      <c r="C45" s="35" t="s">
+        <v>48</v>
       </c>
       <c r="D45" s="36" t="n">
         <v>5.75</v>
@@ -4324,12 +4205,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="46">
-      <c r="A46" s="34" t="n">
+      <c r="A46" s="33" t="n">
         <v>36</v>
       </c>
-      <c r="B46" s="35" t="n"/>
-      <c r="C46" s="30" t="s">
-        <v>50</v>
+      <c r="B46" s="34" t="n"/>
+      <c r="C46" s="35" t="s">
+        <v>49</v>
       </c>
       <c r="D46" s="36" t="n">
         <v>4.5</v>
@@ -4345,12 +4226,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="47">
-      <c r="A47" s="34" t="n">
+      <c r="A47" s="33" t="n">
         <v>37</v>
       </c>
-      <c r="B47" s="35" t="n"/>
-      <c r="C47" s="30" t="s">
-        <v>51</v>
+      <c r="B47" s="34" t="n"/>
+      <c r="C47" s="35" t="s">
+        <v>50</v>
       </c>
       <c r="D47" s="36" t="n">
         <v>4.5</v>
@@ -4366,12 +4247,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="48">
-      <c r="A48" s="34" t="n">
+      <c r="A48" s="33" t="n">
         <v>38</v>
       </c>
-      <c r="B48" s="35" t="n"/>
-      <c r="C48" s="30" t="s">
-        <v>52</v>
+      <c r="B48" s="34" t="n"/>
+      <c r="C48" s="35" t="s">
+        <v>51</v>
       </c>
       <c r="D48" s="36" t="n">
         <v>4.5</v>
@@ -4387,12 +4268,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="49">
-      <c r="A49" s="34" t="n">
+      <c r="A49" s="33" t="n">
         <v>39</v>
       </c>
-      <c r="B49" s="35" t="n"/>
-      <c r="C49" s="30" t="s">
-        <v>53</v>
+      <c r="B49" s="34" t="n"/>
+      <c r="C49" s="35" t="s">
+        <v>52</v>
       </c>
       <c r="D49" s="36" t="n">
         <v>4.5</v>
@@ -4408,12 +4289,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="50">
-      <c r="A50" s="34" t="n">
+      <c r="A50" s="33" t="n">
         <v>40</v>
       </c>
-      <c r="B50" s="35" t="n"/>
-      <c r="C50" s="30" t="s">
-        <v>54</v>
+      <c r="B50" s="34" t="n"/>
+      <c r="C50" s="35" t="s">
+        <v>53</v>
       </c>
       <c r="D50" s="36" t="n">
         <v>4.5</v>
@@ -4429,12 +4310,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="51">
-      <c r="A51" s="34" t="n">
+      <c r="A51" s="33" t="n">
         <v>41</v>
       </c>
-      <c r="B51" s="35" t="n"/>
-      <c r="C51" s="30" t="s">
-        <v>55</v>
+      <c r="B51" s="34" t="n"/>
+      <c r="C51" s="35" t="s">
+        <v>54</v>
       </c>
       <c r="D51" s="36" t="n">
         <v>4.5</v>
@@ -4450,12 +4331,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="52">
-      <c r="A52" s="34" t="n">
+      <c r="A52" s="33" t="n">
         <v>42</v>
       </c>
-      <c r="B52" s="35" t="n"/>
-      <c r="C52" s="30" t="s">
-        <v>56</v>
+      <c r="B52" s="34" t="n"/>
+      <c r="C52" s="35" t="s">
+        <v>55</v>
       </c>
       <c r="D52" s="36" t="n">
         <v>4.5</v>
@@ -4471,12 +4352,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="53">
-      <c r="A53" s="34" t="n">
+      <c r="A53" s="33" t="n">
         <v>43</v>
       </c>
-      <c r="B53" s="35" t="n"/>
-      <c r="C53" s="30" t="s">
-        <v>57</v>
+      <c r="B53" s="34" t="n"/>
+      <c r="C53" s="35" t="s">
+        <v>56</v>
       </c>
       <c r="D53" s="36" t="n">
         <v>5</v>
@@ -4492,12 +4373,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="54">
-      <c r="A54" s="34" t="n">
+      <c r="A54" s="33" t="n">
         <v>44</v>
       </c>
-      <c r="B54" s="35" t="n"/>
-      <c r="C54" s="30" t="s">
-        <v>58</v>
+      <c r="B54" s="34" t="n"/>
+      <c r="C54" s="35" t="s">
+        <v>57</v>
       </c>
       <c r="D54" s="36" t="n">
         <v>7</v>
@@ -4513,12 +4394,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="55">
-      <c r="A55" s="34" t="n">
+      <c r="A55" s="33" t="n">
         <v>45</v>
       </c>
-      <c r="B55" s="35" t="n"/>
-      <c r="C55" s="30" t="s">
-        <v>59</v>
+      <c r="B55" s="34" t="n"/>
+      <c r="C55" s="35" t="s">
+        <v>58</v>
       </c>
       <c r="D55" s="36" t="n">
         <v>6.5</v>
@@ -4534,12 +4415,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="56">
-      <c r="A56" s="34" t="n">
+      <c r="A56" s="33" t="n">
         <v>46</v>
       </c>
-      <c r="B56" s="35" t="n"/>
-      <c r="C56" s="30" t="s">
-        <v>60</v>
+      <c r="B56" s="34" t="n"/>
+      <c r="C56" s="35" t="s">
+        <v>59</v>
       </c>
       <c r="D56" s="36" t="n">
         <v>4.5</v>
@@ -4555,12 +4436,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="57">
-      <c r="A57" s="34" t="n">
+      <c r="A57" s="33" t="n">
         <v>47</v>
       </c>
-      <c r="B57" s="35" t="n"/>
-      <c r="C57" s="30" t="s">
-        <v>61</v>
+      <c r="B57" s="34" t="n"/>
+      <c r="C57" s="35" t="s">
+        <v>60</v>
       </c>
       <c r="D57" s="36" t="n">
         <v>4.5</v>
@@ -4576,12 +4457,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="58">
-      <c r="A58" s="34" t="n">
+      <c r="A58" s="33" t="n">
         <v>48</v>
       </c>
-      <c r="B58" s="35" t="n"/>
-      <c r="C58" s="30" t="s">
-        <v>62</v>
+      <c r="B58" s="34" t="n"/>
+      <c r="C58" s="35" t="s">
+        <v>61</v>
       </c>
       <c r="D58" s="36" t="n">
         <v>5.25</v>
@@ -4597,12 +4478,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="59">
-      <c r="A59" s="34" t="n">
+      <c r="A59" s="33" t="n">
         <v>49</v>
       </c>
-      <c r="B59" s="35" t="n"/>
-      <c r="C59" s="30" t="s">
-        <v>63</v>
+      <c r="B59" s="34" t="n"/>
+      <c r="C59" s="35" t="s">
+        <v>62</v>
       </c>
       <c r="D59" s="36" t="n">
         <v>4.75</v>
@@ -4618,12 +4499,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="60">
-      <c r="A60" s="34" t="n">
+      <c r="A60" s="33" t="n">
         <v>50</v>
       </c>
-      <c r="B60" s="35" t="n"/>
-      <c r="C60" s="30" t="s">
-        <v>64</v>
+      <c r="B60" s="34" t="n"/>
+      <c r="C60" s="35" t="s">
+        <v>63</v>
       </c>
       <c r="D60" s="36" t="n">
         <v>4.5</v>
@@ -4639,12 +4520,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="61">
-      <c r="A61" s="34" t="n">
+      <c r="A61" s="33" t="n">
         <v>51</v>
       </c>
-      <c r="B61" s="35" t="n"/>
-      <c r="C61" s="30" t="s">
-        <v>65</v>
+      <c r="B61" s="34" t="n"/>
+      <c r="C61" s="35" t="s">
+        <v>64</v>
       </c>
       <c r="D61" s="36" t="n">
         <v>4.75</v>
@@ -4660,12 +4541,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="62">
-      <c r="A62" s="34" t="n">
+      <c r="A62" s="33" t="n">
         <v>52</v>
       </c>
-      <c r="B62" s="35" t="n"/>
-      <c r="C62" s="30" t="s">
-        <v>66</v>
+      <c r="B62" s="34" t="n"/>
+      <c r="C62" s="35" t="s">
+        <v>65</v>
       </c>
       <c r="D62" s="36" t="n">
         <v>4.5</v>
@@ -4681,12 +4562,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="63">
-      <c r="A63" s="34" t="n">
+      <c r="A63" s="33" t="n">
         <v>53</v>
       </c>
-      <c r="B63" s="35" t="n"/>
-      <c r="C63" s="30" t="s">
-        <v>67</v>
+      <c r="B63" s="34" t="n"/>
+      <c r="C63" s="35" t="s">
+        <v>66</v>
       </c>
       <c r="D63" s="36" t="n">
         <v>7</v>
@@ -4702,12 +4583,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="64">
-      <c r="A64" s="34" t="n">
+      <c r="A64" s="33" t="n">
         <v>54</v>
       </c>
-      <c r="B64" s="35" t="n"/>
-      <c r="C64" s="30" t="s">
-        <v>68</v>
+      <c r="B64" s="34" t="n"/>
+      <c r="C64" s="35" t="s">
+        <v>67</v>
       </c>
       <c r="D64" s="36" t="n">
         <v>6.75</v>
@@ -4723,12 +4604,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="65">
-      <c r="A65" s="34" t="n">
+      <c r="A65" s="33" t="n">
         <v>55</v>
       </c>
-      <c r="B65" s="35" t="n"/>
-      <c r="C65" s="30" t="s">
-        <v>69</v>
+      <c r="B65" s="34" t="n"/>
+      <c r="C65" s="35" t="s">
+        <v>68</v>
       </c>
       <c r="D65" s="36" t="n">
         <v>4.75</v>
@@ -4744,12 +4625,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="66">
-      <c r="A66" s="34" t="n">
+      <c r="A66" s="33" t="n">
         <v>56</v>
       </c>
-      <c r="B66" s="35" t="n"/>
-      <c r="C66" s="30" t="s">
-        <v>70</v>
+      <c r="B66" s="34" t="n"/>
+      <c r="C66" s="35" t="s">
+        <v>69</v>
       </c>
       <c r="D66" s="36" t="n">
         <v>7</v>
@@ -4765,12 +4646,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="67">
-      <c r="A67" s="34" t="n">
+      <c r="A67" s="33" t="n">
         <v>57</v>
       </c>
-      <c r="B67" s="35" t="n"/>
-      <c r="C67" s="30" t="s">
-        <v>71</v>
+      <c r="B67" s="34" t="n"/>
+      <c r="C67" s="35" t="s">
+        <v>70</v>
       </c>
       <c r="D67" s="36" t="n">
         <v>5.5</v>
@@ -4786,12 +4667,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="68">
-      <c r="A68" s="34" t="n">
+      <c r="A68" s="33" t="n">
         <v>58</v>
       </c>
-      <c r="B68" s="35" t="n"/>
-      <c r="C68" s="30" t="s">
-        <v>72</v>
+      <c r="B68" s="34" t="n"/>
+      <c r="C68" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="D68" s="36" t="n">
         <v>5</v>
@@ -4807,12 +4688,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="69">
-      <c r="A69" s="34" t="n">
+      <c r="A69" s="33" t="n">
         <v>59</v>
       </c>
-      <c r="B69" s="35" t="n"/>
-      <c r="C69" s="30" t="s">
-        <v>73</v>
+      <c r="B69" s="34" t="n"/>
+      <c r="C69" s="35" t="s">
+        <v>72</v>
       </c>
       <c r="D69" s="36" t="n">
         <v>4.5</v>
@@ -4828,12 +4709,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="70">
-      <c r="A70" s="34" t="n">
+      <c r="A70" s="33" t="n">
         <v>60</v>
       </c>
-      <c r="B70" s="35" t="n"/>
-      <c r="C70" s="30" t="s">
-        <v>74</v>
+      <c r="B70" s="34" t="n"/>
+      <c r="C70" s="35" t="s">
+        <v>73</v>
       </c>
       <c r="D70" s="36" t="n">
         <v>4.5</v>
@@ -4849,12 +4730,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="71">
-      <c r="A71" s="34" t="n">
+      <c r="A71" s="33" t="n">
         <v>61</v>
       </c>
-      <c r="B71" s="35" t="n"/>
-      <c r="C71" s="30" t="s">
-        <v>75</v>
+      <c r="B71" s="34" t="n"/>
+      <c r="C71" s="35" t="s">
+        <v>74</v>
       </c>
       <c r="D71" s="36" t="n">
         <v>6.75</v>
@@ -4870,12 +4751,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="72">
-      <c r="A72" s="34" t="n">
+      <c r="A72" s="33" t="n">
         <v>62</v>
       </c>
-      <c r="B72" s="35" t="n"/>
-      <c r="C72" s="30" t="s">
-        <v>76</v>
+      <c r="B72" s="34" t="n"/>
+      <c r="C72" s="35" t="s">
+        <v>75</v>
       </c>
       <c r="D72" s="36" t="n">
         <v>4.5</v>
@@ -4891,12 +4772,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="73">
-      <c r="A73" s="34" t="n">
+      <c r="A73" s="33" t="n">
         <v>63</v>
       </c>
-      <c r="B73" s="35" t="n"/>
-      <c r="C73" s="30" t="s">
-        <v>77</v>
+      <c r="B73" s="34" t="n"/>
+      <c r="C73" s="35" t="s">
+        <v>76</v>
       </c>
       <c r="D73" s="36" t="n">
         <v>4.5</v>
@@ -4912,12 +4793,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="74">
-      <c r="A74" s="34" t="n">
+      <c r="A74" s="33" t="n">
         <v>64</v>
       </c>
-      <c r="B74" s="35" t="n"/>
-      <c r="C74" s="30" t="s">
-        <v>78</v>
+      <c r="B74" s="34" t="n"/>
+      <c r="C74" s="35" t="s">
+        <v>77</v>
       </c>
       <c r="D74" s="36" t="n">
         <v>6</v>
@@ -4933,12 +4814,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="75">
-      <c r="A75" s="34" t="n">
+      <c r="A75" s="33" t="n">
         <v>65</v>
       </c>
-      <c r="B75" s="35" t="n"/>
-      <c r="C75" s="30" t="s">
-        <v>79</v>
+      <c r="B75" s="34" t="n"/>
+      <c r="C75" s="35" t="s">
+        <v>78</v>
       </c>
       <c r="D75" s="36" t="n">
         <v>7</v>
@@ -4954,12 +4835,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="76">
-      <c r="A76" s="34" t="n">
+      <c r="A76" s="33" t="n">
         <v>66</v>
       </c>
-      <c r="B76" s="35" t="n"/>
-      <c r="C76" s="30" t="s">
-        <v>80</v>
+      <c r="B76" s="34" t="n"/>
+      <c r="C76" s="35" t="s">
+        <v>79</v>
       </c>
       <c r="D76" s="36" t="n">
         <v>4.5</v>
@@ -4975,12 +4856,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="77">
-      <c r="A77" s="34" t="n">
+      <c r="A77" s="33" t="n">
         <v>67</v>
       </c>
-      <c r="B77" s="35" t="n"/>
-      <c r="C77" s="30" t="s">
-        <v>81</v>
+      <c r="B77" s="34" t="n"/>
+      <c r="C77" s="35" t="s">
+        <v>80</v>
       </c>
       <c r="D77" s="36" t="n">
         <v>4.5</v>
@@ -4996,12 +4877,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="78">
-      <c r="A78" s="34" t="n">
+      <c r="A78" s="33" t="n">
         <v>68</v>
       </c>
-      <c r="B78" s="35" t="n"/>
-      <c r="C78" s="30" t="s">
-        <v>82</v>
+      <c r="B78" s="34" t="n"/>
+      <c r="C78" s="35" t="s">
+        <v>81</v>
       </c>
       <c r="D78" s="36" t="n">
         <v>4.5</v>
@@ -5017,12 +4898,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="79">
-      <c r="A79" s="34" t="n">
+      <c r="A79" s="33" t="n">
         <v>69</v>
       </c>
-      <c r="B79" s="35" t="n"/>
-      <c r="C79" s="30" t="s">
-        <v>83</v>
+      <c r="B79" s="34" t="n"/>
+      <c r="C79" s="35" t="s">
+        <v>82</v>
       </c>
       <c r="D79" s="36" t="n">
         <v>4.75</v>
@@ -5038,12 +4919,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="80">
-      <c r="A80" s="34" t="n">
+      <c r="A80" s="33" t="n">
         <v>70</v>
       </c>
-      <c r="B80" s="35" t="n"/>
-      <c r="C80" s="30" t="s">
-        <v>84</v>
+      <c r="B80" s="34" t="n"/>
+      <c r="C80" s="35" t="s">
+        <v>83</v>
       </c>
       <c r="D80" s="36" t="n">
         <v>4.5</v>
@@ -5059,12 +4940,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="81">
-      <c r="A81" s="34" t="n">
+      <c r="A81" s="33" t="n">
         <v>71</v>
       </c>
-      <c r="B81" s="35" t="n"/>
-      <c r="C81" s="30" t="s">
-        <v>85</v>
+      <c r="B81" s="34" t="n"/>
+      <c r="C81" s="35" t="s">
+        <v>84</v>
       </c>
       <c r="D81" s="36" t="n">
         <v>7</v>
@@ -5080,12 +4961,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="82">
-      <c r="A82" s="34" t="n">
+      <c r="A82" s="33" t="n">
         <v>72</v>
       </c>
-      <c r="B82" s="35" t="n"/>
-      <c r="C82" s="30" t="s">
-        <v>86</v>
+      <c r="B82" s="34" t="n"/>
+      <c r="C82" s="35" t="s">
+        <v>85</v>
       </c>
       <c r="D82" s="36" t="n">
         <v>7</v>
@@ -5101,12 +4982,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="83">
-      <c r="A83" s="34" t="n">
+      <c r="A83" s="33" t="n">
         <v>73</v>
       </c>
-      <c r="B83" s="35" t="n"/>
-      <c r="C83" s="30" t="s">
-        <v>87</v>
+      <c r="B83" s="34" t="n"/>
+      <c r="C83" s="35" t="s">
+        <v>86</v>
       </c>
       <c r="D83" s="36" t="n">
         <v>5.75</v>
@@ -5122,12 +5003,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="84">
-      <c r="A84" s="34" t="n">
+      <c r="A84" s="33" t="n">
         <v>74</v>
       </c>
-      <c r="B84" s="35" t="n"/>
-      <c r="C84" s="30" t="s">
-        <v>88</v>
+      <c r="B84" s="34" t="n"/>
+      <c r="C84" s="35" t="s">
+        <v>87</v>
       </c>
       <c r="D84" s="36" t="n">
         <v>7</v>
@@ -5143,12 +5024,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="85">
-      <c r="A85" s="34" t="n">
+      <c r="A85" s="33" t="n">
         <v>75</v>
       </c>
-      <c r="B85" s="35" t="n"/>
-      <c r="C85" s="30" t="s">
-        <v>89</v>
+      <c r="B85" s="34" t="n"/>
+      <c r="C85" s="35" t="s">
+        <v>88</v>
       </c>
       <c r="D85" s="36" t="n">
         <v>4.5</v>
@@ -5164,12 +5045,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="86">
-      <c r="A86" s="34" t="n">
+      <c r="A86" s="33" t="n">
         <v>76</v>
       </c>
-      <c r="B86" s="35" t="n"/>
-      <c r="C86" s="30" t="s">
-        <v>90</v>
+      <c r="B86" s="34" t="n"/>
+      <c r="C86" s="35" t="s">
+        <v>89</v>
       </c>
       <c r="D86" s="36" t="n">
         <v>4.5</v>
@@ -5185,12 +5066,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="87">
-      <c r="A87" s="34" t="n">
+      <c r="A87" s="33" t="n">
         <v>77</v>
       </c>
-      <c r="B87" s="35" t="n"/>
-      <c r="C87" s="30" t="s">
-        <v>91</v>
+      <c r="B87" s="34" t="n"/>
+      <c r="C87" s="35" t="s">
+        <v>90</v>
       </c>
       <c r="D87" s="36" t="n">
         <v>6.75</v>
@@ -5206,12 +5087,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="88">
-      <c r="A88" s="34" t="n">
+      <c r="A88" s="33" t="n">
         <v>78</v>
       </c>
-      <c r="B88" s="35" t="n"/>
-      <c r="C88" s="30" t="s">
-        <v>92</v>
+      <c r="B88" s="34" t="n"/>
+      <c r="C88" s="35" t="s">
+        <v>91</v>
       </c>
       <c r="D88" s="36" t="n">
         <v>4.5</v>
@@ -5227,12 +5108,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="89">
-      <c r="A89" s="34" t="n">
+      <c r="A89" s="33" t="n">
         <v>79</v>
       </c>
-      <c r="B89" s="35" t="n"/>
-      <c r="C89" s="30" t="s">
-        <v>93</v>
+      <c r="B89" s="34" t="n"/>
+      <c r="C89" s="35" t="s">
+        <v>92</v>
       </c>
       <c r="D89" s="36" t="n">
         <v>4.75</v>
@@ -5248,12 +5129,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="90">
-      <c r="A90" s="34" t="n">
+      <c r="A90" s="33" t="n">
         <v>80</v>
       </c>
-      <c r="B90" s="35" t="n"/>
-      <c r="C90" s="30" t="s">
-        <v>94</v>
+      <c r="B90" s="34" t="n"/>
+      <c r="C90" s="35" t="s">
+        <v>93</v>
       </c>
       <c r="D90" s="36" t="n">
         <v>4.5</v>
@@ -5269,12 +5150,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="91">
-      <c r="A91" s="34" t="n">
+      <c r="A91" s="33" t="n">
         <v>81</v>
       </c>
-      <c r="B91" s="35" t="n"/>
-      <c r="C91" s="30" t="s">
-        <v>95</v>
+      <c r="B91" s="34" t="n"/>
+      <c r="C91" s="35" t="s">
+        <v>94</v>
       </c>
       <c r="D91" s="36" t="n">
         <v>4.5</v>
@@ -5290,33 +5171,33 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="92">
-      <c r="A92" s="34" t="n">
+      <c r="A92" s="33" t="n">
         <v>82</v>
       </c>
-      <c r="B92" s="35" t="n"/>
-      <c r="C92" s="30" t="s">
+      <c r="B92" s="34" t="n"/>
+      <c r="C92" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D92" s="40" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="E92" s="40" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="F92" s="40" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="G92" s="40" t="n">
+        <v>44.5</v>
+      </c>
+    </row>
+    <row customHeight="true" ht="13.5" outlineLevel="0" r="93">
+      <c r="A93" s="33" t="n">
+        <v>83</v>
+      </c>
+      <c r="B93" s="34" t="n"/>
+      <c r="C93" s="35" t="s">
         <v>96</v>
-      </c>
-      <c r="D92" s="36" t="n">
-        <v>6.25</v>
-      </c>
-      <c r="E92" s="36" t="n">
-        <v>44.5</v>
-      </c>
-      <c r="F92" s="36" t="n">
-        <v>6.25</v>
-      </c>
-      <c r="G92" s="36" t="n">
-        <v>44.5</v>
-      </c>
-    </row>
-    <row customHeight="true" ht="13.5" outlineLevel="0" r="93">
-      <c r="A93" s="34" t="n">
-        <v>83</v>
-      </c>
-      <c r="B93" s="35" t="n"/>
-      <c r="C93" s="30" t="s">
-        <v>97</v>
       </c>
       <c r="D93" s="36" t="n">
         <v>5.75</v>
@@ -5332,12 +5213,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="94">
-      <c r="A94" s="34" t="n">
+      <c r="A94" s="33" t="n">
         <v>84</v>
       </c>
-      <c r="B94" s="35" t="n"/>
-      <c r="C94" s="30" t="s">
-        <v>98</v>
+      <c r="B94" s="34" t="n"/>
+      <c r="C94" s="35" t="s">
+        <v>97</v>
       </c>
       <c r="D94" s="36" t="n">
         <v>7</v>
@@ -5353,12 +5234,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="95">
-      <c r="A95" s="34" t="n">
+      <c r="A95" s="33" t="n">
         <v>85</v>
       </c>
-      <c r="B95" s="35" t="n"/>
-      <c r="C95" s="30" t="s">
-        <v>99</v>
+      <c r="B95" s="34" t="n"/>
+      <c r="C95" s="35" t="s">
+        <v>98</v>
       </c>
       <c r="D95" s="36" t="n">
         <v>4.5</v>
@@ -5374,12 +5255,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="96">
-      <c r="A96" s="34" t="n">
+      <c r="A96" s="33" t="n">
         <v>86</v>
       </c>
-      <c r="B96" s="35" t="n"/>
-      <c r="C96" s="30" t="s">
-        <v>100</v>
+      <c r="B96" s="34" t="n"/>
+      <c r="C96" s="35" t="s">
+        <v>99</v>
       </c>
       <c r="D96" s="36" t="n">
         <v>4.5</v>
@@ -5395,12 +5276,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="97">
-      <c r="A97" s="34" t="n">
+      <c r="A97" s="33" t="n">
         <v>87</v>
       </c>
-      <c r="B97" s="35" t="n"/>
-      <c r="C97" s="30" t="s">
-        <v>101</v>
+      <c r="B97" s="34" t="n"/>
+      <c r="C97" s="35" t="s">
+        <v>100</v>
       </c>
       <c r="D97" s="36" t="n">
         <v>4.5</v>
@@ -5416,12 +5297,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="98">
-      <c r="A98" s="34" t="n">
+      <c r="A98" s="33" t="n">
         <v>88</v>
       </c>
-      <c r="B98" s="35" t="n"/>
-      <c r="C98" s="30" t="s">
-        <v>102</v>
+      <c r="B98" s="34" t="n"/>
+      <c r="C98" s="35" t="s">
+        <v>101</v>
       </c>
       <c r="D98" s="36" t="n">
         <v>4.5</v>
@@ -5437,12 +5318,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="99">
-      <c r="A99" s="34" t="n">
+      <c r="A99" s="33" t="n">
         <v>89</v>
       </c>
-      <c r="B99" s="35" t="n"/>
-      <c r="C99" s="30" t="s">
-        <v>103</v>
+      <c r="B99" s="34" t="n"/>
+      <c r="C99" s="35" t="s">
+        <v>102</v>
       </c>
       <c r="D99" s="36" t="n">
         <v>4.5</v>
@@ -5458,12 +5339,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="100">
-      <c r="A100" s="34" t="n">
+      <c r="A100" s="33" t="n">
         <v>90</v>
       </c>
-      <c r="B100" s="35" t="n"/>
-      <c r="C100" s="30" t="s">
-        <v>104</v>
+      <c r="B100" s="34" t="n"/>
+      <c r="C100" s="35" t="s">
+        <v>103</v>
       </c>
       <c r="D100" s="36" t="n">
         <v>6.75</v>
@@ -5479,12 +5360,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="101">
-      <c r="A101" s="34" t="n">
+      <c r="A101" s="33" t="n">
         <v>91</v>
       </c>
-      <c r="B101" s="35" t="n"/>
-      <c r="C101" s="30" t="s">
-        <v>105</v>
+      <c r="B101" s="34" t="n"/>
+      <c r="C101" s="35" t="s">
+        <v>104</v>
       </c>
       <c r="D101" s="36" t="n">
         <v>4.5</v>
@@ -5500,12 +5381,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="102">
-      <c r="A102" s="34" t="n">
+      <c r="A102" s="33" t="n">
         <v>92</v>
       </c>
-      <c r="B102" s="35" t="n"/>
-      <c r="C102" s="30" t="s">
-        <v>106</v>
+      <c r="B102" s="34" t="n"/>
+      <c r="C102" s="35" t="s">
+        <v>105</v>
       </c>
       <c r="D102" s="36" t="n">
         <v>4.5</v>
@@ -5521,12 +5402,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="103">
-      <c r="A103" s="34" t="n">
+      <c r="A103" s="33" t="n">
         <v>93</v>
       </c>
-      <c r="B103" s="35" t="n"/>
-      <c r="C103" s="30" t="s">
-        <v>107</v>
+      <c r="B103" s="34" t="n"/>
+      <c r="C103" s="35" t="s">
+        <v>106</v>
       </c>
       <c r="D103" s="36" t="n">
         <v>4.75</v>
@@ -5542,12 +5423,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="104">
-      <c r="A104" s="34" t="n">
+      <c r="A104" s="33" t="n">
         <v>94</v>
       </c>
-      <c r="B104" s="35" t="n"/>
-      <c r="C104" s="30" t="s">
-        <v>108</v>
+      <c r="B104" s="34" t="n"/>
+      <c r="C104" s="35" t="s">
+        <v>107</v>
       </c>
       <c r="D104" s="36" t="n">
         <v>4.5</v>
@@ -5563,12 +5444,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="105">
-      <c r="A105" s="34" t="n">
+      <c r="A105" s="33" t="n">
         <v>95</v>
       </c>
-      <c r="B105" s="35" t="n"/>
-      <c r="C105" s="30" t="s">
-        <v>109</v>
+      <c r="B105" s="34" t="n"/>
+      <c r="C105" s="35" t="s">
+        <v>108</v>
       </c>
       <c r="D105" s="36" t="n">
         <v>5</v>
@@ -5584,12 +5465,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="106">
-      <c r="A106" s="34" t="n">
+      <c r="A106" s="33" t="n">
         <v>96</v>
       </c>
-      <c r="B106" s="35" t="n"/>
-      <c r="C106" s="30" t="s">
-        <v>110</v>
+      <c r="B106" s="34" t="n"/>
+      <c r="C106" s="35" t="s">
+        <v>109</v>
       </c>
       <c r="D106" s="36" t="n">
         <v>4.5</v>
@@ -5605,12 +5486,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="107">
-      <c r="A107" s="34" t="n">
+      <c r="A107" s="33" t="n">
         <v>97</v>
       </c>
-      <c r="B107" s="35" t="n"/>
-      <c r="C107" s="30" t="s">
-        <v>111</v>
+      <c r="B107" s="34" t="n"/>
+      <c r="C107" s="35" t="s">
+        <v>110</v>
       </c>
       <c r="D107" s="36" t="n">
         <v>4.5</v>
@@ -5626,12 +5507,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="108">
-      <c r="A108" s="34" t="n">
+      <c r="A108" s="33" t="n">
         <v>98</v>
       </c>
-      <c r="B108" s="35" t="n"/>
-      <c r="C108" s="30" t="s">
-        <v>112</v>
+      <c r="B108" s="34" t="n"/>
+      <c r="C108" s="35" t="s">
+        <v>111</v>
       </c>
       <c r="D108" s="36" t="n">
         <v>4.5</v>
@@ -5647,12 +5528,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="109">
-      <c r="A109" s="34" t="n">
+      <c r="A109" s="33" t="n">
         <v>99</v>
       </c>
-      <c r="B109" s="35" t="n"/>
-      <c r="C109" s="30" t="s">
-        <v>113</v>
+      <c r="B109" s="34" t="n"/>
+      <c r="C109" s="35" t="s">
+        <v>112</v>
       </c>
       <c r="D109" s="36" t="n">
         <v>4.5</v>
@@ -5668,12 +5549,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="110">
-      <c r="A110" s="34" t="n">
+      <c r="A110" s="33" t="n">
         <v>100</v>
       </c>
-      <c r="B110" s="35" t="n"/>
-      <c r="C110" s="30" t="s">
-        <v>114</v>
+      <c r="B110" s="34" t="n"/>
+      <c r="C110" s="35" t="s">
+        <v>113</v>
       </c>
       <c r="D110" s="36" t="n">
         <v>4.75</v>
@@ -5689,12 +5570,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="111">
-      <c r="A111" s="34" t="n">
+      <c r="A111" s="33" t="n">
         <v>101</v>
       </c>
-      <c r="B111" s="35" t="n"/>
-      <c r="C111" s="30" t="s">
-        <v>115</v>
+      <c r="B111" s="34" t="n"/>
+      <c r="C111" s="35" t="s">
+        <v>114</v>
       </c>
       <c r="D111" s="36" t="n">
         <v>6.75</v>
@@ -5710,12 +5591,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="112">
-      <c r="A112" s="34" t="n">
+      <c r="A112" s="33" t="n">
         <v>102</v>
       </c>
-      <c r="B112" s="35" t="n"/>
-      <c r="C112" s="30" t="s">
-        <v>116</v>
+      <c r="B112" s="34" t="n"/>
+      <c r="C112" s="35" t="s">
+        <v>115</v>
       </c>
       <c r="D112" s="36" t="n">
         <v>4.5</v>
@@ -5731,12 +5612,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="113">
-      <c r="A113" s="34" t="n">
+      <c r="A113" s="33" t="n">
         <v>103</v>
       </c>
-      <c r="B113" s="35" t="n"/>
-      <c r="C113" s="30" t="s">
-        <v>117</v>
+      <c r="B113" s="34" t="n"/>
+      <c r="C113" s="35" t="s">
+        <v>116</v>
       </c>
       <c r="D113" s="36" t="n">
         <v>4.5</v>
@@ -5752,12 +5633,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="114">
-      <c r="A114" s="34" t="n">
+      <c r="A114" s="33" t="n">
         <v>104</v>
       </c>
-      <c r="B114" s="35" t="n"/>
-      <c r="C114" s="30" t="s">
-        <v>118</v>
+      <c r="B114" s="34" t="n"/>
+      <c r="C114" s="35" t="s">
+        <v>117</v>
       </c>
       <c r="D114" s="36" t="n">
         <v>4.5</v>
@@ -5773,12 +5654,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="115">
-      <c r="A115" s="34" t="n">
+      <c r="A115" s="33" t="n">
         <v>105</v>
       </c>
-      <c r="B115" s="35" t="n"/>
-      <c r="C115" s="30" t="s">
-        <v>119</v>
+      <c r="B115" s="34" t="n"/>
+      <c r="C115" s="35" t="s">
+        <v>118</v>
       </c>
       <c r="D115" s="36" t="n">
         <v>4.5</v>
@@ -5794,12 +5675,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="116">
-      <c r="A116" s="34" t="n">
+      <c r="A116" s="33" t="n">
         <v>106</v>
       </c>
-      <c r="B116" s="35" t="n"/>
-      <c r="C116" s="30" t="s">
-        <v>120</v>
+      <c r="B116" s="34" t="n"/>
+      <c r="C116" s="35" t="s">
+        <v>119</v>
       </c>
       <c r="D116" s="36" t="n">
         <v>5.25</v>
@@ -5815,12 +5696,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="117">
-      <c r="A117" s="34" t="n">
+      <c r="A117" s="33" t="n">
         <v>107</v>
       </c>
-      <c r="B117" s="35" t="n"/>
-      <c r="C117" s="30" t="s">
-        <v>121</v>
+      <c r="B117" s="34" t="n"/>
+      <c r="C117" s="35" t="s">
+        <v>120</v>
       </c>
       <c r="D117" s="36" t="n">
         <v>6.5</v>
@@ -5836,12 +5717,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="118">
-      <c r="A118" s="34" t="n">
+      <c r="A118" s="33" t="n">
         <v>108</v>
       </c>
-      <c r="B118" s="35" t="n"/>
-      <c r="C118" s="30" t="s">
-        <v>122</v>
+      <c r="B118" s="34" t="n"/>
+      <c r="C118" s="35" t="s">
+        <v>121</v>
       </c>
       <c r="D118" s="36" t="n">
         <v>6.5</v>
@@ -5857,12 +5738,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="119">
-      <c r="A119" s="34" t="n">
+      <c r="A119" s="33" t="n">
         <v>109</v>
       </c>
-      <c r="B119" s="35" t="n"/>
-      <c r="C119" s="30" t="s">
-        <v>123</v>
+      <c r="B119" s="34" t="n"/>
+      <c r="C119" s="35" t="s">
+        <v>122</v>
       </c>
       <c r="D119" s="36" t="n">
         <v>4.5</v>
@@ -5878,12 +5759,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="120">
-      <c r="A120" s="34" t="n">
+      <c r="A120" s="33" t="n">
         <v>110</v>
       </c>
-      <c r="B120" s="35" t="n"/>
-      <c r="C120" s="30" t="s">
-        <v>124</v>
+      <c r="B120" s="34" t="n"/>
+      <c r="C120" s="35" t="s">
+        <v>123</v>
       </c>
       <c r="D120" s="36" t="n">
         <v>4.5</v>
@@ -5899,12 +5780,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="121">
-      <c r="A121" s="34" t="n">
+      <c r="A121" s="33" t="n">
         <v>111</v>
       </c>
-      <c r="B121" s="35" t="n"/>
-      <c r="C121" s="30" t="s">
-        <v>125</v>
+      <c r="B121" s="34" t="n"/>
+      <c r="C121" s="35" t="s">
+        <v>124</v>
       </c>
       <c r="D121" s="36" t="n">
         <v>4.5</v>
@@ -5920,12 +5801,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="122">
-      <c r="A122" s="34" t="n">
+      <c r="A122" s="33" t="n">
         <v>112</v>
       </c>
-      <c r="B122" s="35" t="n"/>
-      <c r="C122" s="30" t="s">
-        <v>126</v>
+      <c r="B122" s="34" t="n"/>
+      <c r="C122" s="35" t="s">
+        <v>125</v>
       </c>
       <c r="D122" s="36" t="n">
         <v>7</v>
@@ -5941,12 +5822,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="123">
-      <c r="A123" s="34" t="n">
+      <c r="A123" s="33" t="n">
         <v>113</v>
       </c>
-      <c r="B123" s="35" t="n"/>
-      <c r="C123" s="30" t="s">
-        <v>127</v>
+      <c r="B123" s="34" t="n"/>
+      <c r="C123" s="35" t="s">
+        <v>126</v>
       </c>
       <c r="D123" s="36" t="n">
         <v>4.75</v>
@@ -5962,12 +5843,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="124">
-      <c r="A124" s="34" t="n">
+      <c r="A124" s="33" t="n">
         <v>114</v>
       </c>
-      <c r="B124" s="35" t="n"/>
-      <c r="C124" s="30" t="s">
-        <v>128</v>
+      <c r="B124" s="34" t="n"/>
+      <c r="C124" s="35" t="s">
+        <v>127</v>
       </c>
       <c r="D124" s="36" t="n">
         <v>5.25</v>
@@ -5983,12 +5864,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="125">
-      <c r="A125" s="34" t="n">
+      <c r="A125" s="33" t="n">
         <v>115</v>
       </c>
-      <c r="B125" s="35" t="n"/>
-      <c r="C125" s="30" t="s">
-        <v>129</v>
+      <c r="B125" s="34" t="n"/>
+      <c r="C125" s="35" t="s">
+        <v>128</v>
       </c>
       <c r="D125" s="36" t="n">
         <v>4.5</v>
@@ -6004,12 +5885,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="126">
-      <c r="A126" s="34" t="n">
+      <c r="A126" s="33" t="n">
         <v>116</v>
       </c>
-      <c r="B126" s="35" t="n"/>
-      <c r="C126" s="30" t="s">
-        <v>130</v>
+      <c r="B126" s="34" t="n"/>
+      <c r="C126" s="35" t="s">
+        <v>129</v>
       </c>
       <c r="D126" s="36" t="n">
         <v>4.75</v>
@@ -6025,12 +5906,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="127">
-      <c r="A127" s="34" t="n">
+      <c r="A127" s="33" t="n">
         <v>117</v>
       </c>
-      <c r="B127" s="35" t="n"/>
-      <c r="C127" s="30" t="s">
-        <v>131</v>
+      <c r="B127" s="34" t="n"/>
+      <c r="C127" s="35" t="s">
+        <v>130</v>
       </c>
       <c r="D127" s="36" t="n">
         <v>4.5</v>
@@ -6046,12 +5927,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="128">
-      <c r="A128" s="34" t="n">
+      <c r="A128" s="33" t="n">
         <v>118</v>
       </c>
-      <c r="B128" s="35" t="n"/>
-      <c r="C128" s="30" t="s">
-        <v>132</v>
+      <c r="B128" s="34" t="n"/>
+      <c r="C128" s="35" t="s">
+        <v>131</v>
       </c>
       <c r="D128" s="36" t="n">
         <v>6.75</v>
@@ -6067,12 +5948,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="129">
-      <c r="A129" s="34" t="n">
+      <c r="A129" s="33" t="n">
         <v>119</v>
       </c>
-      <c r="B129" s="35" t="n"/>
-      <c r="C129" s="30" t="s">
-        <v>133</v>
+      <c r="B129" s="34" t="n"/>
+      <c r="C129" s="35" t="s">
+        <v>132</v>
       </c>
       <c r="D129" s="36" t="n">
         <v>4.75</v>
@@ -6088,12 +5969,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="130">
-      <c r="A130" s="34" t="n">
+      <c r="A130" s="33" t="n">
         <v>120</v>
       </c>
-      <c r="B130" s="35" t="n"/>
-      <c r="C130" s="30" t="s">
-        <v>134</v>
+      <c r="B130" s="34" t="n"/>
+      <c r="C130" s="35" t="s">
+        <v>133</v>
       </c>
       <c r="D130" s="36" t="n">
         <v>4.75</v>
@@ -6109,12 +5990,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="131">
-      <c r="A131" s="34" t="n">
+      <c r="A131" s="33" t="n">
         <v>121</v>
       </c>
-      <c r="B131" s="35" t="n"/>
-      <c r="C131" s="30" t="s">
-        <v>135</v>
+      <c r="B131" s="34" t="n"/>
+      <c r="C131" s="35" t="s">
+        <v>134</v>
       </c>
       <c r="D131" s="36" t="n">
         <v>7</v>
@@ -6130,12 +6011,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="132">
-      <c r="A132" s="34" t="n">
+      <c r="A132" s="33" t="n">
         <v>122</v>
       </c>
-      <c r="B132" s="35" t="n"/>
-      <c r="C132" s="30" t="s">
-        <v>136</v>
+      <c r="B132" s="34" t="n"/>
+      <c r="C132" s="35" t="s">
+        <v>135</v>
       </c>
       <c r="D132" s="36" t="n">
         <v>4.5</v>
@@ -6151,12 +6032,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="133">
-      <c r="A133" s="34" t="n">
+      <c r="A133" s="33" t="n">
         <v>123</v>
       </c>
-      <c r="B133" s="35" t="n"/>
-      <c r="C133" s="30" t="s">
-        <v>137</v>
+      <c r="B133" s="34" t="n"/>
+      <c r="C133" s="35" t="s">
+        <v>136</v>
       </c>
       <c r="D133" s="36" t="n">
         <v>4.5</v>
@@ -6172,12 +6053,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="134">
-      <c r="A134" s="34" t="n">
+      <c r="A134" s="33" t="n">
         <v>124</v>
       </c>
-      <c r="B134" s="35" t="n"/>
-      <c r="C134" s="30" t="s">
-        <v>138</v>
+      <c r="B134" s="34" t="n"/>
+      <c r="C134" s="35" t="s">
+        <v>137</v>
       </c>
       <c r="D134" s="36" t="n">
         <v>4.5</v>
@@ -6193,12 +6074,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="135">
-      <c r="A135" s="34" t="n">
+      <c r="A135" s="33" t="n">
         <v>125</v>
       </c>
-      <c r="B135" s="35" t="n"/>
-      <c r="C135" s="30" t="s">
-        <v>139</v>
+      <c r="B135" s="34" t="n"/>
+      <c r="C135" s="35" t="s">
+        <v>138</v>
       </c>
       <c r="D135" s="36" t="n">
         <v>6.75</v>
@@ -6214,12 +6095,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="136">
-      <c r="A136" s="34" t="n">
+      <c r="A136" s="33" t="n">
         <v>126</v>
       </c>
-      <c r="B136" s="35" t="n"/>
-      <c r="C136" s="30" t="s">
-        <v>140</v>
+      <c r="B136" s="34" t="n"/>
+      <c r="C136" s="35" t="s">
+        <v>139</v>
       </c>
       <c r="D136" s="36" t="n">
         <v>4.5</v>
@@ -6235,12 +6116,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="137">
-      <c r="A137" s="34" t="n">
+      <c r="A137" s="33" t="n">
         <v>127</v>
       </c>
-      <c r="B137" s="35" t="n"/>
-      <c r="C137" s="30" t="s">
-        <v>141</v>
+      <c r="B137" s="34" t="n"/>
+      <c r="C137" s="35" t="s">
+        <v>140</v>
       </c>
       <c r="D137" s="36" t="n">
         <v>5.5</v>
@@ -6256,12 +6137,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="138">
-      <c r="A138" s="34" t="n">
+      <c r="A138" s="33" t="n">
         <v>128</v>
       </c>
-      <c r="B138" s="35" t="n"/>
-      <c r="C138" s="30" t="s">
-        <v>142</v>
+      <c r="B138" s="34" t="n"/>
+      <c r="C138" s="35" t="s">
+        <v>141</v>
       </c>
       <c r="D138" s="36" t="n">
         <v>4.5</v>
@@ -6277,12 +6158,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="139">
-      <c r="A139" s="34" t="n">
+      <c r="A139" s="33" t="n">
         <v>129</v>
       </c>
-      <c r="B139" s="35" t="n"/>
-      <c r="C139" s="30" t="s">
-        <v>143</v>
+      <c r="B139" s="34" t="n"/>
+      <c r="C139" s="35" t="s">
+        <v>142</v>
       </c>
       <c r="D139" s="36" t="n">
         <v>4.5</v>
@@ -6298,12 +6179,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="140">
-      <c r="A140" s="34" t="n">
+      <c r="A140" s="33" t="n">
         <v>130</v>
       </c>
-      <c r="B140" s="35" t="n"/>
-      <c r="C140" s="30" t="s">
-        <v>144</v>
+      <c r="B140" s="34" t="n"/>
+      <c r="C140" s="35" t="s">
+        <v>143</v>
       </c>
       <c r="D140" s="36" t="n">
         <v>4.5</v>
@@ -6319,12 +6200,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="141">
-      <c r="A141" s="34" t="n">
+      <c r="A141" s="33" t="n">
         <v>131</v>
       </c>
-      <c r="B141" s="35" t="n"/>
-      <c r="C141" s="30" t="s">
-        <v>145</v>
+      <c r="B141" s="34" t="n"/>
+      <c r="C141" s="35" t="s">
+        <v>144</v>
       </c>
       <c r="D141" s="36" t="n">
         <v>4.5</v>
@@ -6340,12 +6221,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="142">
-      <c r="A142" s="34" t="n">
+      <c r="A142" s="33" t="n">
         <v>132</v>
       </c>
-      <c r="B142" s="35" t="n"/>
-      <c r="C142" s="30" t="s">
-        <v>146</v>
+      <c r="B142" s="34" t="n"/>
+      <c r="C142" s="35" t="s">
+        <v>145</v>
       </c>
       <c r="D142" s="36" t="n">
         <v>4.5</v>
@@ -6361,12 +6242,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="143">
-      <c r="A143" s="34" t="n">
+      <c r="A143" s="33" t="n">
         <v>133</v>
       </c>
-      <c r="B143" s="35" t="n"/>
-      <c r="C143" s="30" t="s">
-        <v>147</v>
+      <c r="B143" s="34" t="n"/>
+      <c r="C143" s="35" t="s">
+        <v>146</v>
       </c>
       <c r="D143" s="36" t="n">
         <v>4.5</v>
@@ -6382,12 +6263,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="144">
-      <c r="A144" s="34" t="n">
+      <c r="A144" s="33" t="n">
         <v>134</v>
       </c>
-      <c r="B144" s="35" t="n"/>
-      <c r="C144" s="30" t="s">
-        <v>148</v>
+      <c r="B144" s="34" t="n"/>
+      <c r="C144" s="35" t="s">
+        <v>147</v>
       </c>
       <c r="D144" s="36" t="n">
         <v>7</v>
@@ -6403,12 +6284,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="145">
-      <c r="A145" s="34" t="n">
+      <c r="A145" s="33" t="n">
         <v>135</v>
       </c>
-      <c r="B145" s="35" t="n"/>
-      <c r="C145" s="30" t="s">
-        <v>149</v>
+      <c r="B145" s="34" t="n"/>
+      <c r="C145" s="35" t="s">
+        <v>148</v>
       </c>
       <c r="D145" s="36" t="n">
         <v>4.5</v>
@@ -6424,12 +6305,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="146">
-      <c r="A146" s="34" t="n">
+      <c r="A146" s="33" t="n">
         <v>136</v>
       </c>
-      <c r="B146" s="35" t="n"/>
-      <c r="C146" s="30" t="s">
-        <v>150</v>
+      <c r="B146" s="34" t="n"/>
+      <c r="C146" s="35" t="s">
+        <v>149</v>
       </c>
       <c r="D146" s="36" t="n">
         <v>5.75</v>
@@ -6445,12 +6326,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="147">
-      <c r="A147" s="34" t="n">
+      <c r="A147" s="33" t="n">
         <v>137</v>
       </c>
-      <c r="B147" s="35" t="n"/>
-      <c r="C147" s="30" t="s">
-        <v>151</v>
+      <c r="B147" s="34" t="n"/>
+      <c r="C147" s="35" t="s">
+        <v>150</v>
       </c>
       <c r="D147" s="36" t="n">
         <v>6.75</v>
@@ -6466,12 +6347,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="148">
-      <c r="A148" s="34" t="n">
+      <c r="A148" s="33" t="n">
         <v>138</v>
       </c>
-      <c r="B148" s="35" t="n"/>
-      <c r="C148" s="30" t="s">
-        <v>152</v>
+      <c r="B148" s="34" t="n"/>
+      <c r="C148" s="35" t="s">
+        <v>151</v>
       </c>
       <c r="D148" s="36" t="n">
         <v>7</v>
@@ -6487,33 +6368,33 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="149">
-      <c r="A149" s="34" t="n">
+      <c r="A149" s="33" t="n">
         <v>139</v>
       </c>
-      <c r="B149" s="35" t="n"/>
-      <c r="C149" s="40" t="s">
+      <c r="B149" s="34" t="n"/>
+      <c r="C149" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="D149" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="D149" s="28" t="s">
+      <c r="E149" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="F149" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="G149" s="28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row customHeight="true" ht="13.5" outlineLevel="0" r="150">
+      <c r="A150" s="33" t="n">
+        <v>140</v>
+      </c>
+      <c r="B150" s="34" t="n"/>
+      <c r="C150" s="35" t="s">
         <v>154</v>
-      </c>
-      <c r="E149" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="F149" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="G149" s="28" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row customHeight="true" ht="13.5" outlineLevel="0" r="150">
-      <c r="A150" s="34" t="n">
-        <v>140</v>
-      </c>
-      <c r="B150" s="35" t="n"/>
-      <c r="C150" s="30" t="s">
-        <v>155</v>
       </c>
       <c r="D150" s="36" t="n">
         <v>4.5</v>
@@ -6529,12 +6410,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="151">
-      <c r="A151" s="34" t="n">
+      <c r="A151" s="33" t="n">
         <v>141</v>
       </c>
-      <c r="B151" s="35" t="n"/>
-      <c r="C151" s="30" t="s">
-        <v>156</v>
+      <c r="B151" s="34" t="n"/>
+      <c r="C151" s="35" t="s">
+        <v>155</v>
       </c>
       <c r="D151" s="36" t="n">
         <v>5.75</v>
@@ -6550,12 +6431,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="152">
-      <c r="A152" s="34" t="n">
+      <c r="A152" s="33" t="n">
         <v>142</v>
       </c>
-      <c r="B152" s="35" t="n"/>
-      <c r="C152" s="30" t="s">
-        <v>157</v>
+      <c r="B152" s="34" t="n"/>
+      <c r="C152" s="35" t="s">
+        <v>156</v>
       </c>
       <c r="D152" s="36" t="n">
         <v>4.5</v>
@@ -6571,33 +6452,33 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="153">
-      <c r="A153" s="34" t="n">
+      <c r="A153" s="33" t="n">
         <v>143</v>
       </c>
-      <c r="B153" s="35" t="n"/>
-      <c r="C153" s="30" t="s">
+      <c r="B153" s="34" t="n"/>
+      <c r="C153" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="D153" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="E153" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="F153" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="G153" s="28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row customHeight="true" ht="13.5" outlineLevel="0" r="154">
+      <c r="A154" s="33" t="n">
+        <v>144</v>
+      </c>
+      <c r="B154" s="34" t="n"/>
+      <c r="C154" s="35" t="s">
         <v>158</v>
-      </c>
-      <c r="D153" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="E153" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="F153" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="G153" s="28" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row customHeight="true" ht="13.5" outlineLevel="0" r="154">
-      <c r="A154" s="34" t="n">
-        <v>144</v>
-      </c>
-      <c r="B154" s="35" t="n"/>
-      <c r="C154" s="30" t="s">
-        <v>159</v>
       </c>
       <c r="D154" s="36" t="n">
         <v>4.5</v>
@@ -6613,12 +6494,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="155">
-      <c r="A155" s="34" t="n">
+      <c r="A155" s="33" t="n">
         <v>145</v>
       </c>
-      <c r="B155" s="35" t="n"/>
-      <c r="C155" s="30" t="s">
-        <v>160</v>
+      <c r="B155" s="34" t="n"/>
+      <c r="C155" s="35" t="s">
+        <v>159</v>
       </c>
       <c r="D155" s="36" t="n">
         <v>4.5</v>
@@ -6634,12 +6515,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="156">
-      <c r="A156" s="34" t="n">
+      <c r="A156" s="33" t="n">
         <v>146</v>
       </c>
-      <c r="B156" s="35" t="n"/>
-      <c r="C156" s="30" t="s">
-        <v>161</v>
+      <c r="B156" s="34" t="n"/>
+      <c r="C156" s="35" t="s">
+        <v>160</v>
       </c>
       <c r="D156" s="36" t="n">
         <v>4.5</v>
@@ -6655,12 +6536,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="157">
-      <c r="A157" s="34" t="n">
+      <c r="A157" s="33" t="n">
         <v>147</v>
       </c>
-      <c r="B157" s="35" t="n"/>
-      <c r="C157" s="30" t="s">
-        <v>162</v>
+      <c r="B157" s="34" t="n"/>
+      <c r="C157" s="35" t="s">
+        <v>161</v>
       </c>
       <c r="D157" s="36" t="n">
         <v>6</v>
@@ -6676,12 +6557,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="158">
-      <c r="A158" s="34" t="n">
+      <c r="A158" s="33" t="n">
         <v>148</v>
       </c>
-      <c r="B158" s="35" t="n"/>
-      <c r="C158" s="30" t="s">
-        <v>163</v>
+      <c r="B158" s="34" t="n"/>
+      <c r="C158" s="35" t="s">
+        <v>162</v>
       </c>
       <c r="D158" s="36" t="n">
         <v>4.5</v>
@@ -6697,12 +6578,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="159">
-      <c r="A159" s="34" t="n">
+      <c r="A159" s="33" t="n">
         <v>149</v>
       </c>
-      <c r="B159" s="35" t="n"/>
-      <c r="C159" s="30" t="s">
-        <v>164</v>
+      <c r="B159" s="34" t="n"/>
+      <c r="C159" s="35" t="s">
+        <v>163</v>
       </c>
       <c r="D159" s="36" t="n">
         <v>6</v>
@@ -6718,12 +6599,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="160">
-      <c r="A160" s="34" t="n">
+      <c r="A160" s="33" t="n">
         <v>150</v>
       </c>
-      <c r="B160" s="35" t="n"/>
-      <c r="C160" s="30" t="s">
-        <v>165</v>
+      <c r="B160" s="34" t="n"/>
+      <c r="C160" s="35" t="s">
+        <v>164</v>
       </c>
       <c r="D160" s="36" t="n">
         <v>6.75</v>
@@ -6739,12 +6620,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="161">
-      <c r="A161" s="34" t="n">
+      <c r="A161" s="33" t="n">
         <v>151</v>
       </c>
-      <c r="B161" s="35" t="n"/>
-      <c r="C161" s="30" t="s">
-        <v>166</v>
+      <c r="B161" s="34" t="n"/>
+      <c r="C161" s="35" t="s">
+        <v>165</v>
       </c>
       <c r="D161" s="36" t="n">
         <v>7</v>
@@ -6760,12 +6641,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="162">
-      <c r="A162" s="34" t="n">
+      <c r="A162" s="33" t="n">
         <v>152</v>
       </c>
-      <c r="B162" s="35" t="n"/>
-      <c r="C162" s="30" t="s">
-        <v>167</v>
+      <c r="B162" s="34" t="n"/>
+      <c r="C162" s="35" t="s">
+        <v>166</v>
       </c>
       <c r="D162" s="36" t="n">
         <v>6.25</v>
@@ -6781,12 +6662,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="163">
-      <c r="A163" s="34" t="n">
+      <c r="A163" s="33" t="n">
         <v>153</v>
       </c>
-      <c r="B163" s="35" t="n"/>
-      <c r="C163" s="30" t="s">
-        <v>168</v>
+      <c r="B163" s="34" t="n"/>
+      <c r="C163" s="35" t="s">
+        <v>167</v>
       </c>
       <c r="D163" s="36" t="n">
         <v>4.5</v>
@@ -6802,12 +6683,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="164">
-      <c r="A164" s="34" t="n">
+      <c r="A164" s="33" t="n">
         <v>154</v>
       </c>
-      <c r="B164" s="35" t="n"/>
-      <c r="C164" s="30" t="s">
-        <v>169</v>
+      <c r="B164" s="34" t="n"/>
+      <c r="C164" s="35" t="s">
+        <v>168</v>
       </c>
       <c r="D164" s="36" t="n">
         <v>5</v>
@@ -6823,12 +6704,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="165">
-      <c r="A165" s="34" t="n">
+      <c r="A165" s="33" t="n">
         <v>155</v>
       </c>
-      <c r="B165" s="35" t="n"/>
-      <c r="C165" s="30" t="s">
-        <v>170</v>
+      <c r="B165" s="34" t="n"/>
+      <c r="C165" s="35" t="s">
+        <v>169</v>
       </c>
       <c r="D165" s="36" t="n">
         <v>6</v>
@@ -6844,12 +6725,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="166">
-      <c r="A166" s="34" t="n">
+      <c r="A166" s="33" t="n">
         <v>156</v>
       </c>
-      <c r="B166" s="35" t="n"/>
-      <c r="C166" s="30" t="s">
-        <v>171</v>
+      <c r="B166" s="34" t="n"/>
+      <c r="C166" s="35" t="s">
+        <v>170</v>
       </c>
       <c r="D166" s="36" t="n">
         <v>4.5</v>
@@ -6865,12 +6746,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="167">
-      <c r="A167" s="34" t="n">
+      <c r="A167" s="33" t="n">
         <v>157</v>
       </c>
-      <c r="B167" s="35" t="n"/>
-      <c r="C167" s="30" t="s">
-        <v>172</v>
+      <c r="B167" s="34" t="n"/>
+      <c r="C167" s="35" t="s">
+        <v>171</v>
       </c>
       <c r="D167" s="36" t="n">
         <v>4.5</v>
@@ -6886,12 +6767,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="168">
-      <c r="A168" s="34" t="n">
+      <c r="A168" s="33" t="n">
         <v>158</v>
       </c>
-      <c r="B168" s="35" t="n"/>
-      <c r="C168" s="30" t="s">
-        <v>173</v>
+      <c r="B168" s="34" t="n"/>
+      <c r="C168" s="35" t="s">
+        <v>172</v>
       </c>
       <c r="D168" s="36" t="n">
         <v>6</v>
@@ -6907,12 +6788,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="169">
-      <c r="A169" s="34" t="n">
+      <c r="A169" s="33" t="n">
         <v>159</v>
       </c>
-      <c r="B169" s="35" t="n"/>
-      <c r="C169" s="30" t="s">
-        <v>174</v>
+      <c r="B169" s="34" t="n"/>
+      <c r="C169" s="35" t="s">
+        <v>173</v>
       </c>
       <c r="D169" s="36" t="n">
         <v>6.75</v>
@@ -6928,12 +6809,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="170">
-      <c r="A170" s="34" t="n">
+      <c r="A170" s="33" t="n">
         <v>160</v>
       </c>
-      <c r="B170" s="35" t="n"/>
-      <c r="C170" s="30" t="s">
-        <v>175</v>
+      <c r="B170" s="34" t="n"/>
+      <c r="C170" s="35" t="s">
+        <v>174</v>
       </c>
       <c r="D170" s="36" t="n">
         <v>4.75</v>
@@ -6949,12 +6830,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="171">
-      <c r="A171" s="34" t="n">
+      <c r="A171" s="33" t="n">
         <v>161</v>
       </c>
-      <c r="B171" s="35" t="n"/>
-      <c r="C171" s="30" t="s">
-        <v>176</v>
+      <c r="B171" s="34" t="n"/>
+      <c r="C171" s="35" t="s">
+        <v>175</v>
       </c>
       <c r="D171" s="36" t="n">
         <v>4.5</v>
@@ -6970,12 +6851,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="172">
-      <c r="A172" s="34" t="n">
+      <c r="A172" s="33" t="n">
         <v>162</v>
       </c>
-      <c r="B172" s="35" t="n"/>
-      <c r="C172" s="30" t="s">
-        <v>177</v>
+      <c r="B172" s="34" t="n"/>
+      <c r="C172" s="35" t="s">
+        <v>176</v>
       </c>
       <c r="D172" s="36" t="n">
         <v>7</v>
@@ -6991,12 +6872,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="173">
-      <c r="A173" s="34" t="n">
+      <c r="A173" s="33" t="n">
         <v>163</v>
       </c>
-      <c r="B173" s="35" t="n"/>
-      <c r="C173" s="30" t="s">
-        <v>178</v>
+      <c r="B173" s="34" t="n"/>
+      <c r="C173" s="35" t="s">
+        <v>177</v>
       </c>
       <c r="D173" s="36" t="n">
         <v>4.5</v>
@@ -7012,12 +6893,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="174">
-      <c r="A174" s="34" t="n">
+      <c r="A174" s="33" t="n">
         <v>164</v>
       </c>
-      <c r="B174" s="35" t="n"/>
-      <c r="C174" s="30" t="s">
-        <v>179</v>
+      <c r="B174" s="34" t="n"/>
+      <c r="C174" s="35" t="s">
+        <v>178</v>
       </c>
       <c r="D174" s="36" t="n">
         <v>5</v>
@@ -7033,12 +6914,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="175">
-      <c r="A175" s="34" t="n">
+      <c r="A175" s="33" t="n">
         <v>165</v>
       </c>
-      <c r="B175" s="35" t="n"/>
-      <c r="C175" s="30" t="s">
-        <v>180</v>
+      <c r="B175" s="34" t="n"/>
+      <c r="C175" s="35" t="s">
+        <v>179</v>
       </c>
       <c r="D175" s="36" t="n">
         <v>4.5</v>
@@ -7054,12 +6935,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="176">
-      <c r="A176" s="34" t="n">
+      <c r="A176" s="33" t="n">
         <v>166</v>
       </c>
-      <c r="B176" s="35" t="n"/>
-      <c r="C176" s="30" t="s">
-        <v>181</v>
+      <c r="B176" s="34" t="n"/>
+      <c r="C176" s="35" t="s">
+        <v>180</v>
       </c>
       <c r="D176" s="36" t="n">
         <v>4.5</v>
@@ -7075,12 +6956,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="177">
-      <c r="A177" s="34" t="n">
+      <c r="A177" s="33" t="n">
         <v>167</v>
       </c>
-      <c r="B177" s="35" t="n"/>
-      <c r="C177" s="30" t="s">
-        <v>182</v>
+      <c r="B177" s="34" t="n"/>
+      <c r="C177" s="35" t="s">
+        <v>181</v>
       </c>
       <c r="D177" s="36" t="n">
         <v>4.5</v>
@@ -7096,12 +6977,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="178">
-      <c r="A178" s="34" t="n">
+      <c r="A178" s="33" t="n">
         <v>168</v>
       </c>
-      <c r="B178" s="31" t="n"/>
-      <c r="C178" s="30" t="s">
-        <v>183</v>
+      <c r="B178" s="30" t="n"/>
+      <c r="C178" s="35" t="s">
+        <v>182</v>
       </c>
       <c r="D178" s="36" t="n">
         <v>4.5</v>
@@ -7117,12 +6998,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="179">
-      <c r="A179" s="34" t="n">
+      <c r="A179" s="33" t="n">
         <v>169</v>
       </c>
-      <c r="B179" s="35" t="n"/>
-      <c r="C179" s="30" t="s">
-        <v>184</v>
+      <c r="B179" s="34" t="n"/>
+      <c r="C179" s="35" t="s">
+        <v>183</v>
       </c>
       <c r="D179" s="36" t="n">
         <v>4.75</v>
@@ -7138,33 +7019,33 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="180">
-      <c r="A180" s="34" t="n">
+      <c r="A180" s="33" t="n">
         <v>170</v>
       </c>
-      <c r="B180" s="35" t="n"/>
-      <c r="C180" s="30" t="s">
+      <c r="B180" s="34" t="n"/>
+      <c r="C180" s="35" t="s">
+        <v>184</v>
+      </c>
+      <c r="D180" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="E180" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="F180" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="G180" s="28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row customHeight="true" ht="13.5" outlineLevel="0" r="181">
+      <c r="A181" s="33" t="n">
+        <v>171</v>
+      </c>
+      <c r="B181" s="34" t="n"/>
+      <c r="C181" s="35" t="s">
         <v>185</v>
-      </c>
-      <c r="D180" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="E180" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="F180" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="G180" s="28" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row customHeight="true" ht="13.5" outlineLevel="0" r="181">
-      <c r="A181" s="34" t="n">
-        <v>171</v>
-      </c>
-      <c r="B181" s="35" t="n"/>
-      <c r="C181" s="30" t="s">
-        <v>186</v>
       </c>
       <c r="D181" s="36" t="n">
         <v>6</v>
@@ -7180,12 +7061,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="182">
-      <c r="A182" s="34" t="n">
+      <c r="A182" s="33" t="n">
         <v>172</v>
       </c>
-      <c r="B182" s="35" t="n"/>
-      <c r="C182" s="30" t="s">
-        <v>187</v>
+      <c r="B182" s="34" t="n"/>
+      <c r="C182" s="35" t="s">
+        <v>186</v>
       </c>
       <c r="D182" s="36" t="n">
         <v>6</v>
@@ -7201,12 +7082,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="183">
-      <c r="A183" s="34" t="n">
+      <c r="A183" s="33" t="n">
         <v>173</v>
       </c>
-      <c r="B183" s="35" t="n"/>
-      <c r="C183" s="30" t="s">
-        <v>188</v>
+      <c r="B183" s="34" t="n"/>
+      <c r="C183" s="35" t="s">
+        <v>187</v>
       </c>
       <c r="D183" s="36" t="n">
         <v>4.5</v>
@@ -7222,33 +7103,33 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="184">
-      <c r="A184" s="34" t="n">
+      <c r="A184" s="33" t="n">
         <v>174</v>
       </c>
-      <c r="B184" s="35" t="n"/>
-      <c r="C184" s="30" t="s">
+      <c r="B184" s="34" t="n"/>
+      <c r="C184" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="D184" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="E184" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="F184" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="G184" s="28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row customHeight="true" ht="13.5" outlineLevel="0" r="185">
+      <c r="A185" s="33" t="n">
+        <v>175</v>
+      </c>
+      <c r="B185" s="34" t="n"/>
+      <c r="C185" s="35" t="s">
         <v>189</v>
-      </c>
-      <c r="D184" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="E184" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="F184" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="G184" s="28" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row customHeight="true" ht="13.5" outlineLevel="0" r="185">
-      <c r="A185" s="34" t="n">
-        <v>175</v>
-      </c>
-      <c r="B185" s="35" t="n"/>
-      <c r="C185" s="30" t="s">
-        <v>190</v>
       </c>
       <c r="D185" s="36" t="n">
         <v>4.5</v>
@@ -7264,12 +7145,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="186">
-      <c r="A186" s="34" t="n">
+      <c r="A186" s="33" t="n">
         <v>176</v>
       </c>
-      <c r="B186" s="35" t="n"/>
-      <c r="C186" s="30" t="s">
-        <v>191</v>
+      <c r="B186" s="34" t="n"/>
+      <c r="C186" s="35" t="s">
+        <v>190</v>
       </c>
       <c r="D186" s="36" t="n">
         <v>5.5</v>
@@ -7285,12 +7166,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="187">
-      <c r="A187" s="34" t="n">
+      <c r="A187" s="33" t="n">
         <v>177</v>
       </c>
-      <c r="B187" s="35" t="n"/>
-      <c r="C187" s="30" t="s">
-        <v>192</v>
+      <c r="B187" s="34" t="n"/>
+      <c r="C187" s="35" t="s">
+        <v>191</v>
       </c>
       <c r="D187" s="36" t="n">
         <v>5.25</v>
@@ -7306,12 +7187,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="188">
-      <c r="A188" s="34" t="n">
+      <c r="A188" s="33" t="n">
         <v>178</v>
       </c>
-      <c r="B188" s="35" t="n"/>
-      <c r="C188" s="30" t="s">
-        <v>193</v>
+      <c r="B188" s="34" t="n"/>
+      <c r="C188" s="35" t="s">
+        <v>192</v>
       </c>
       <c r="D188" s="36" t="n">
         <v>4.5</v>
@@ -7327,12 +7208,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="189">
-      <c r="A189" s="34" t="n">
+      <c r="A189" s="33" t="n">
         <v>179</v>
       </c>
-      <c r="B189" s="35" t="n"/>
-      <c r="C189" s="30" t="s">
-        <v>194</v>
+      <c r="B189" s="34" t="n"/>
+      <c r="C189" s="35" t="s">
+        <v>193</v>
       </c>
       <c r="D189" s="36" t="n">
         <v>4.5</v>
@@ -7348,12 +7229,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="190">
-      <c r="A190" s="34" t="n">
+      <c r="A190" s="33" t="n">
         <v>180</v>
       </c>
-      <c r="B190" s="35" t="n"/>
-      <c r="C190" s="30" t="s">
-        <v>195</v>
+      <c r="B190" s="34" t="n"/>
+      <c r="C190" s="35" t="s">
+        <v>194</v>
       </c>
       <c r="D190" s="36" t="n">
         <v>4.75</v>
@@ -7369,12 +7250,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="191">
-      <c r="A191" s="34" t="n">
+      <c r="A191" s="33" t="n">
         <v>181</v>
       </c>
-      <c r="B191" s="35" t="n"/>
-      <c r="C191" s="30" t="s">
-        <v>196</v>
+      <c r="B191" s="34" t="n"/>
+      <c r="C191" s="35" t="s">
+        <v>195</v>
       </c>
       <c r="D191" s="36" t="n">
         <v>5</v>
@@ -7390,12 +7271,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="192">
-      <c r="A192" s="34" t="n">
+      <c r="A192" s="33" t="n">
         <v>182</v>
       </c>
-      <c r="B192" s="35" t="n"/>
-      <c r="C192" s="30" t="s">
-        <v>197</v>
+      <c r="B192" s="34" t="n"/>
+      <c r="C192" s="35" t="s">
+        <v>196</v>
       </c>
       <c r="D192" s="36" t="n">
         <v>4.5</v>
@@ -7411,12 +7292,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="193">
-      <c r="A193" s="34" t="n">
+      <c r="A193" s="33" t="n">
         <v>183</v>
       </c>
-      <c r="B193" s="35" t="n"/>
-      <c r="C193" s="30" t="s">
-        <v>198</v>
+      <c r="B193" s="34" t="n"/>
+      <c r="C193" s="35" t="s">
+        <v>197</v>
       </c>
       <c r="D193" s="36" t="n">
         <v>4.5</v>
@@ -7432,12 +7313,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="194">
-      <c r="A194" s="34" t="n">
+      <c r="A194" s="33" t="n">
         <v>184</v>
       </c>
-      <c r="B194" s="35" t="n"/>
-      <c r="C194" s="30" t="s">
-        <v>199</v>
+      <c r="B194" s="34" t="n"/>
+      <c r="C194" s="35" t="s">
+        <v>198</v>
       </c>
       <c r="D194" s="36" t="n">
         <v>4.75</v>
@@ -7453,12 +7334,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="195">
-      <c r="A195" s="34" t="n">
+      <c r="A195" s="33" t="n">
         <v>185</v>
       </c>
-      <c r="B195" s="35" t="n"/>
-      <c r="C195" s="30" t="s">
-        <v>200</v>
+      <c r="B195" s="34" t="n"/>
+      <c r="C195" s="35" t="s">
+        <v>199</v>
       </c>
       <c r="D195" s="36" t="n">
         <v>4.5</v>
@@ -7474,12 +7355,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="196">
-      <c r="A196" s="34" t="n">
+      <c r="A196" s="33" t="n">
         <v>186</v>
       </c>
-      <c r="B196" s="35" t="n"/>
-      <c r="C196" s="30" t="s">
-        <v>201</v>
+      <c r="B196" s="34" t="n"/>
+      <c r="C196" s="35" t="s">
+        <v>200</v>
       </c>
       <c r="D196" s="36" t="n">
         <v>4.5</v>
@@ -7495,33 +7376,33 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="197">
-      <c r="A197" s="34" t="n">
+      <c r="A197" s="33" t="n">
         <v>187</v>
       </c>
-      <c r="B197" s="41" t="s">
+      <c r="B197" s="42" t="s">
+        <v>201</v>
+      </c>
+      <c r="C197" s="43" t="s"/>
+      <c r="D197" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="E197" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="F197" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="G197" s="28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row customHeight="true" ht="13.5" outlineLevel="0" r="198">
+      <c r="A198" s="33" t="n">
+        <v>188</v>
+      </c>
+      <c r="B198" s="34" t="n"/>
+      <c r="C198" s="35" t="s">
         <v>202</v>
-      </c>
-      <c r="C197" s="42" t="s"/>
-      <c r="D197" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="E197" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="F197" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="G197" s="28" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row customHeight="true" ht="13.5" outlineLevel="0" r="198">
-      <c r="A198" s="34" t="n">
-        <v>188</v>
-      </c>
-      <c r="B198" s="35" t="n"/>
-      <c r="C198" s="30" t="s">
-        <v>203</v>
       </c>
       <c r="D198" s="36" t="n">
         <v>4.5</v>
@@ -7537,12 +7418,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="199">
-      <c r="A199" s="34" t="n">
+      <c r="A199" s="33" t="n">
         <v>189</v>
       </c>
-      <c r="B199" s="35" t="n"/>
-      <c r="C199" s="30" t="s">
-        <v>204</v>
+      <c r="B199" s="34" t="n"/>
+      <c r="C199" s="35" t="s">
+        <v>203</v>
       </c>
       <c r="D199" s="36" t="n">
         <v>4.5</v>
@@ -7558,12 +7439,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="200">
-      <c r="A200" s="34" t="n">
+      <c r="A200" s="33" t="n">
         <v>190</v>
       </c>
-      <c r="B200" s="35" t="n"/>
-      <c r="C200" s="30" t="s">
-        <v>205</v>
+      <c r="B200" s="34" t="n"/>
+      <c r="C200" s="35" t="s">
+        <v>204</v>
       </c>
       <c r="D200" s="36" t="n">
         <v>5.25</v>
@@ -7579,12 +7460,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="201">
-      <c r="A201" s="34" t="n">
+      <c r="A201" s="33" t="n">
         <v>191</v>
       </c>
-      <c r="B201" s="35" t="n"/>
-      <c r="C201" s="30" t="s">
-        <v>206</v>
+      <c r="B201" s="34" t="n"/>
+      <c r="C201" s="35" t="s">
+        <v>205</v>
       </c>
       <c r="D201" s="36" t="n">
         <v>7</v>
@@ -7600,12 +7481,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="202">
-      <c r="A202" s="34" t="n">
+      <c r="A202" s="33" t="n">
         <v>192</v>
       </c>
-      <c r="B202" s="35" t="n"/>
-      <c r="C202" s="30" t="s">
-        <v>207</v>
+      <c r="B202" s="34" t="n"/>
+      <c r="C202" s="35" t="s">
+        <v>206</v>
       </c>
       <c r="D202" s="36" t="n">
         <v>4.5</v>
@@ -7621,12 +7502,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="203">
-      <c r="A203" s="34" t="n">
+      <c r="A203" s="33" t="n">
         <v>193</v>
       </c>
-      <c r="B203" s="35" t="n"/>
-      <c r="C203" s="30" t="s">
-        <v>208</v>
+      <c r="B203" s="34" t="n"/>
+      <c r="C203" s="35" t="s">
+        <v>207</v>
       </c>
       <c r="D203" s="36" t="n">
         <v>4.5</v>
@@ -7642,33 +7523,33 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="204">
-      <c r="A204" s="34" t="n">
+      <c r="A204" s="33" t="n">
         <v>194</v>
       </c>
-      <c r="B204" s="35" t="n"/>
-      <c r="C204" s="30" t="s">
+      <c r="B204" s="34" t="n"/>
+      <c r="C204" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="D204" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="E204" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="F204" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="G204" s="28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row customHeight="true" ht="13.5" outlineLevel="0" r="205">
+      <c r="A205" s="33" t="n">
+        <v>195</v>
+      </c>
+      <c r="B205" s="34" t="n"/>
+      <c r="C205" s="35" t="s">
         <v>209</v>
-      </c>
-      <c r="D204" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="E204" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="F204" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="G204" s="28" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row customHeight="true" ht="13.5" outlineLevel="0" r="205">
-      <c r="A205" s="34" t="n">
-        <v>195</v>
-      </c>
-      <c r="B205" s="35" t="n"/>
-      <c r="C205" s="30" t="s">
-        <v>210</v>
       </c>
       <c r="D205" s="36" t="n">
         <v>4.5</v>
@@ -7684,12 +7565,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="206">
-      <c r="A206" s="34" t="n">
+      <c r="A206" s="33" t="n">
         <v>196</v>
       </c>
-      <c r="B206" s="35" t="n"/>
-      <c r="C206" s="30" t="s">
-        <v>211</v>
+      <c r="B206" s="34" t="n"/>
+      <c r="C206" s="35" t="s">
+        <v>210</v>
       </c>
       <c r="D206" s="36" t="n">
         <v>4.5</v>
@@ -7705,12 +7586,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="207">
-      <c r="A207" s="34" t="n">
+      <c r="A207" s="33" t="n">
         <v>197</v>
       </c>
-      <c r="B207" s="35" t="n"/>
-      <c r="C207" s="30" t="s">
-        <v>212</v>
+      <c r="B207" s="34" t="n"/>
+      <c r="C207" s="35" t="s">
+        <v>211</v>
       </c>
       <c r="D207" s="36" t="n">
         <v>5.75</v>
@@ -7726,12 +7607,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="208">
-      <c r="A208" s="34" t="n">
+      <c r="A208" s="33" t="n">
         <v>198</v>
       </c>
-      <c r="B208" s="35" t="n"/>
-      <c r="C208" s="30" t="s">
-        <v>213</v>
+      <c r="B208" s="34" t="n"/>
+      <c r="C208" s="35" t="s">
+        <v>212</v>
       </c>
       <c r="D208" s="36" t="n">
         <v>4.5</v>
@@ -7747,12 +7628,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="209">
-      <c r="A209" s="34" t="n">
+      <c r="A209" s="33" t="n">
         <v>199</v>
       </c>
-      <c r="B209" s="35" t="n"/>
-      <c r="C209" s="30" t="s">
-        <v>214</v>
+      <c r="B209" s="34" t="n"/>
+      <c r="C209" s="35" t="s">
+        <v>213</v>
       </c>
       <c r="D209" s="36" t="n">
         <v>4.5</v>
@@ -7768,33 +7649,33 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="210">
-      <c r="A210" s="34" t="n">
+      <c r="A210" s="33" t="n">
         <v>200</v>
       </c>
-      <c r="B210" s="35" t="n"/>
-      <c r="C210" s="30" t="s">
+      <c r="B210" s="34" t="n"/>
+      <c r="C210" s="35" t="s">
+        <v>214</v>
+      </c>
+      <c r="D210" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="E210" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="F210" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="G210" s="28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row customHeight="true" ht="13.5" outlineLevel="0" r="211">
+      <c r="A211" s="33" t="n">
+        <v>201</v>
+      </c>
+      <c r="B211" s="34" t="n"/>
+      <c r="C211" s="35" t="s">
         <v>215</v>
-      </c>
-      <c r="D210" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="E210" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="F210" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="G210" s="28" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row customHeight="true" ht="13.5" outlineLevel="0" r="211">
-      <c r="A211" s="34" t="n">
-        <v>201</v>
-      </c>
-      <c r="B211" s="35" t="n"/>
-      <c r="C211" s="30" t="s">
-        <v>216</v>
       </c>
       <c r="D211" s="36" t="n">
         <v>4.5</v>
@@ -7810,12 +7691,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="212">
-      <c r="A212" s="34" t="n">
+      <c r="A212" s="33" t="n">
         <v>202</v>
       </c>
-      <c r="B212" s="35" t="n"/>
-      <c r="C212" s="30" t="s">
-        <v>217</v>
+      <c r="B212" s="34" t="n"/>
+      <c r="C212" s="35" t="s">
+        <v>216</v>
       </c>
       <c r="D212" s="36" t="n">
         <v>7</v>
@@ -7831,12 +7712,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="213">
-      <c r="A213" s="34" t="n">
+      <c r="A213" s="33" t="n">
         <v>203</v>
       </c>
-      <c r="B213" s="35" t="n"/>
-      <c r="C213" s="30" t="s">
-        <v>218</v>
+      <c r="B213" s="34" t="n"/>
+      <c r="C213" s="35" t="s">
+        <v>217</v>
       </c>
       <c r="D213" s="36" t="n">
         <v>7</v>
@@ -7852,12 +7733,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="214">
-      <c r="A214" s="34" t="n">
+      <c r="A214" s="33" t="n">
         <v>204</v>
       </c>
-      <c r="B214" s="35" t="n"/>
-      <c r="C214" s="30" t="s">
-        <v>219</v>
+      <c r="B214" s="34" t="n"/>
+      <c r="C214" s="35" t="s">
+        <v>218</v>
       </c>
       <c r="D214" s="36" t="n">
         <v>5.75</v>
@@ -7873,12 +7754,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="215">
-      <c r="A215" s="34" t="n">
+      <c r="A215" s="33" t="n">
         <v>205</v>
       </c>
-      <c r="B215" s="35" t="n"/>
-      <c r="C215" s="30" t="s">
-        <v>220</v>
+      <c r="B215" s="34" t="n"/>
+      <c r="C215" s="35" t="s">
+        <v>219</v>
       </c>
       <c r="D215" s="36" t="n">
         <v>5.25</v>
@@ -7894,12 +7775,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="216">
-      <c r="A216" s="34" t="n">
+      <c r="A216" s="33" t="n">
         <v>206</v>
       </c>
-      <c r="B216" s="35" t="n"/>
-      <c r="C216" s="30" t="s">
-        <v>221</v>
+      <c r="B216" s="34" t="n"/>
+      <c r="C216" s="35" t="s">
+        <v>220</v>
       </c>
       <c r="D216" s="36" t="n">
         <v>5.5</v>
@@ -7915,12 +7796,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="217">
-      <c r="A217" s="34" t="n">
+      <c r="A217" s="33" t="n">
         <v>207</v>
       </c>
-      <c r="B217" s="35" t="n"/>
-      <c r="C217" s="30" t="s">
-        <v>222</v>
+      <c r="B217" s="34" t="n"/>
+      <c r="C217" s="35" t="s">
+        <v>221</v>
       </c>
       <c r="D217" s="36" t="n">
         <v>4.5</v>
@@ -7936,12 +7817,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="218">
-      <c r="A218" s="34" t="n">
+      <c r="A218" s="33" t="n">
         <v>208</v>
       </c>
-      <c r="B218" s="35" t="n"/>
-      <c r="C218" s="30" t="s">
-        <v>223</v>
+      <c r="B218" s="34" t="n"/>
+      <c r="C218" s="35" t="s">
+        <v>222</v>
       </c>
       <c r="D218" s="36" t="n">
         <v>4.5</v>
@@ -7957,12 +7838,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="219">
-      <c r="A219" s="34" t="n">
+      <c r="A219" s="33" t="n">
         <v>209</v>
       </c>
-      <c r="B219" s="35" t="n"/>
-      <c r="C219" s="30" t="s">
-        <v>224</v>
+      <c r="B219" s="34" t="n"/>
+      <c r="C219" s="35" t="s">
+        <v>223</v>
       </c>
       <c r="D219" s="36" t="n">
         <v>6.5</v>
@@ -7978,12 +7859,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="220">
-      <c r="A220" s="34" t="n">
+      <c r="A220" s="33" t="n">
         <v>210</v>
       </c>
-      <c r="B220" s="35" t="n"/>
-      <c r="C220" s="30" t="s">
-        <v>225</v>
+      <c r="B220" s="34" t="n"/>
+      <c r="C220" s="35" t="s">
+        <v>224</v>
       </c>
       <c r="D220" s="36" t="n">
         <v>4.5</v>
@@ -7999,12 +7880,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="221">
-      <c r="A221" s="34" t="n">
+      <c r="A221" s="33" t="n">
         <v>211</v>
       </c>
-      <c r="B221" s="35" t="n"/>
-      <c r="C221" s="30" t="s">
-        <v>226</v>
+      <c r="B221" s="34" t="n"/>
+      <c r="C221" s="35" t="s">
+        <v>225</v>
       </c>
       <c r="D221" s="36" t="n">
         <v>6.5</v>
@@ -8020,12 +7901,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="222">
-      <c r="A222" s="34" t="n">
+      <c r="A222" s="33" t="n">
         <v>212</v>
       </c>
-      <c r="B222" s="35" t="n"/>
-      <c r="C222" s="30" t="s">
-        <v>227</v>
+      <c r="B222" s="34" t="n"/>
+      <c r="C222" s="35" t="s">
+        <v>226</v>
       </c>
       <c r="D222" s="36" t="n">
         <v>7</v>
@@ -8041,12 +7922,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="223">
-      <c r="A223" s="34" t="n">
+      <c r="A223" s="33" t="n">
         <v>213</v>
       </c>
-      <c r="B223" s="35" t="n"/>
-      <c r="C223" s="30" t="s">
-        <v>228</v>
+      <c r="B223" s="34" t="n"/>
+      <c r="C223" s="35" t="s">
+        <v>227</v>
       </c>
       <c r="D223" s="36" t="n">
         <v>4.5</v>
@@ -8062,12 +7943,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="224">
-      <c r="A224" s="34" t="n">
+      <c r="A224" s="33" t="n">
         <v>214</v>
       </c>
-      <c r="B224" s="35" t="n"/>
-      <c r="C224" s="30" t="s">
-        <v>229</v>
+      <c r="B224" s="34" t="n"/>
+      <c r="C224" s="35" t="s">
+        <v>228</v>
       </c>
       <c r="D224" s="36" t="n">
         <v>6.75</v>
@@ -8083,12 +7964,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="225">
-      <c r="A225" s="34" t="n">
+      <c r="A225" s="33" t="n">
         <v>215</v>
       </c>
-      <c r="B225" s="35" t="n"/>
-      <c r="C225" s="30" t="s">
-        <v>230</v>
+      <c r="B225" s="34" t="n"/>
+      <c r="C225" s="35" t="s">
+        <v>229</v>
       </c>
       <c r="D225" s="36" t="n">
         <v>5.5</v>
@@ -8104,12 +7985,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="226">
-      <c r="A226" s="34" t="n">
+      <c r="A226" s="33" t="n">
         <v>216</v>
       </c>
-      <c r="B226" s="35" t="n"/>
-      <c r="C226" s="30" t="s">
-        <v>231</v>
+      <c r="B226" s="34" t="n"/>
+      <c r="C226" s="35" t="s">
+        <v>230</v>
       </c>
       <c r="D226" s="36" t="n">
         <v>4.5</v>
@@ -8125,12 +8006,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="227">
-      <c r="A227" s="34" t="n">
+      <c r="A227" s="33" t="n">
         <v>217</v>
       </c>
-      <c r="B227" s="35" t="n"/>
-      <c r="C227" s="30" t="s">
-        <v>232</v>
+      <c r="B227" s="34" t="n"/>
+      <c r="C227" s="35" t="s">
+        <v>231</v>
       </c>
       <c r="D227" s="36" t="n">
         <v>6.75</v>
@@ -8146,12 +8027,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="228">
-      <c r="A228" s="34" t="n">
+      <c r="A228" s="33" t="n">
         <v>218</v>
       </c>
-      <c r="B228" s="35" t="n"/>
-      <c r="C228" s="30" t="s">
-        <v>233</v>
+      <c r="B228" s="34" t="n"/>
+      <c r="C228" s="35" t="s">
+        <v>232</v>
       </c>
       <c r="D228" s="36" t="n">
         <v>4.5</v>
@@ -8167,12 +8048,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="229">
-      <c r="A229" s="34" t="n">
+      <c r="A229" s="33" t="n">
         <v>219</v>
       </c>
-      <c r="B229" s="35" t="n"/>
-      <c r="C229" s="30" t="s">
-        <v>234</v>
+      <c r="B229" s="34" t="n"/>
+      <c r="C229" s="35" t="s">
+        <v>233</v>
       </c>
       <c r="D229" s="36" t="n">
         <v>4.75</v>
@@ -8188,12 +8069,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="230">
-      <c r="A230" s="34" t="n">
+      <c r="A230" s="33" t="n">
         <v>220</v>
       </c>
-      <c r="B230" s="35" t="n"/>
-      <c r="C230" s="30" t="s">
-        <v>235</v>
+      <c r="B230" s="34" t="n"/>
+      <c r="C230" s="35" t="s">
+        <v>234</v>
       </c>
       <c r="D230" s="36" t="n">
         <v>4.5</v>
@@ -8209,12 +8090,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="231">
-      <c r="A231" s="34" t="n">
+      <c r="A231" s="33" t="n">
         <v>221</v>
       </c>
-      <c r="B231" s="35" t="n"/>
-      <c r="C231" s="30" t="s">
-        <v>236</v>
+      <c r="B231" s="34" t="n"/>
+      <c r="C231" s="35" t="s">
+        <v>235</v>
       </c>
       <c r="D231" s="36" t="n">
         <v>4.5</v>
@@ -8230,12 +8111,12 @@
       </c>
     </row>
     <row customHeight="true" ht="13.5" outlineLevel="0" r="232">
-      <c r="A232" s="34" t="n">
+      <c r="A232" s="33" t="n">
         <v>222</v>
       </c>
-      <c r="B232" s="35" t="n"/>
-      <c r="C232" s="30" t="s">
-        <v>237</v>
+      <c r="B232" s="34" t="n"/>
+      <c r="C232" s="35" t="s">
+        <v>236</v>
       </c>
       <c r="D232" s="36" t="n">
         <v>4.75</v>
@@ -8250,174 +8131,133 @@
         <v>27.5</v>
       </c>
     </row>
-    <row customHeight="true" ht="43.75" outlineLevel="0" r="233">
-      <c r="A233" s="34" t="n">
+    <row ht="0" outlineLevel="0" r="233">
+      <c r="A233" s="33" t="n">
         <v>223</v>
       </c>
-      <c r="B233" s="43" t="n"/>
-      <c r="C233" s="30" t="s">
-        <v>238</v>
-      </c>
-      <c r="D233" s="44" t="s"/>
-      <c r="E233" s="45" t="s"/>
-      <c r="F233" s="46" t="s"/>
-      <c r="G233" s="47" t="s"/>
-    </row>
-    <row customHeight="true" ht="38.75" outlineLevel="0" r="234">
+      <c r="B233" s="44" t="n"/>
+      <c r="C233" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="D233" s="45" t="s"/>
+      <c r="E233" s="46" t="s"/>
+      <c r="F233" s="47" t="s"/>
+      <c r="G233" s="48" t="s"/>
+    </row>
+    <row ht="0" outlineLevel="0" r="234">
       <c r="A234" s="37" t="n">
         <v>224</v>
       </c>
-      <c r="B234" s="43" t="n"/>
-      <c r="C234" s="30" t="s">
+      <c r="B234" s="44" t="n"/>
+      <c r="C234" s="35" t="s">
+        <v>238</v>
+      </c>
+      <c r="D234" s="49" t="s"/>
+      <c r="E234" s="50" t="s"/>
+      <c r="F234" s="51" t="s"/>
+      <c r="G234" s="52" t="s"/>
+    </row>
+    <row ht="0" outlineLevel="0" r="235">
+      <c r="A235" s="33" t="n">
+        <v>225</v>
+      </c>
+      <c r="B235" s="44" t="n"/>
+      <c r="C235" s="35" t="s">
         <v>239</v>
       </c>
-      <c r="D234" s="48" t="s"/>
-      <c r="E234" s="49" t="s"/>
-      <c r="F234" s="50" t="s"/>
-      <c r="G234" s="51" t="s"/>
-    </row>
-    <row customHeight="true" ht="41.5" outlineLevel="0" r="235">
-      <c r="A235" s="34" t="n">
-        <v>225</v>
-      </c>
-      <c r="B235" s="43" t="n"/>
-      <c r="C235" s="30" t="s">
+      <c r="D235" s="53" t="s"/>
+      <c r="E235" s="54" t="s"/>
+      <c r="F235" s="55" t="s"/>
+      <c r="G235" s="56" t="s"/>
+    </row>
+    <row customHeight="true" ht="25.24951171875" outlineLevel="0" r="236">
+      <c r="A236" s="44" t="n"/>
+      <c r="B236" s="31" t="n">
+        <v>2</v>
+      </c>
+      <c r="C236" s="32" t="s">
         <v>240</v>
       </c>
-      <c r="D235" s="52" t="s"/>
-      <c r="E235" s="53" t="s"/>
-      <c r="F235" s="54" t="s"/>
-      <c r="G235" s="55" t="s"/>
-    </row>
-    <row customHeight="true" ht="25.24951171875" outlineLevel="0" r="236">
-      <c r="A236" s="43" t="n"/>
-      <c r="B236" s="32" t="n">
-        <v>2</v>
-      </c>
-      <c r="C236" s="33" t="s">
+      <c r="D236" s="44" t="n"/>
+      <c r="E236" s="57" t="s"/>
+      <c r="F236" s="58" t="s">
         <v>241</v>
       </c>
-      <c r="D236" s="43" t="n"/>
-      <c r="E236" s="56" t="s"/>
-      <c r="F236" s="57" t="s">
+      <c r="G236" s="59" t="s"/>
+    </row>
+    <row customHeight="true" ht="41.5" outlineLevel="0" r="237">
+      <c r="A237" s="33" t="n">
+        <v>226</v>
+      </c>
+      <c r="B237" s="44" t="n"/>
+      <c r="C237" s="35" t="s">
         <v>242</v>
       </c>
-      <c r="G236" s="58" t="s"/>
-    </row>
-    <row customHeight="true" ht="41.5" outlineLevel="0" r="237">
-      <c r="A237" s="34" t="n">
-        <v>226</v>
-      </c>
-      <c r="B237" s="43" t="n"/>
-      <c r="C237" s="30" t="s">
+      <c r="D237" s="60" t="s"/>
+      <c r="E237" s="61" t="s"/>
+      <c r="F237" s="62" t="s"/>
+      <c r="G237" s="63" t="s"/>
+    </row>
+    <row customHeight="true" ht="31" outlineLevel="0" r="238">
+      <c r="A238" s="33" t="n">
+        <v>227</v>
+      </c>
+      <c r="B238" s="30" t="n"/>
+      <c r="C238" s="35" t="s">
         <v>243</v>
       </c>
-      <c r="D237" s="59" t="s"/>
-      <c r="E237" s="60" t="s"/>
-      <c r="F237" s="61" t="s"/>
-      <c r="G237" s="62" t="s"/>
-    </row>
-    <row customHeight="true" ht="31" outlineLevel="0" r="238">
-      <c r="A238" s="34" t="n">
-        <v>227</v>
-      </c>
-      <c r="B238" s="31" t="n"/>
-      <c r="C238" s="30" t="s">
-        <v>244</v>
-      </c>
-      <c r="D238" s="63" t="s"/>
-      <c r="E238" s="64" t="s"/>
+      <c r="D238" s="64" t="s"/>
+      <c r="E238" s="65" t="s"/>
       <c r="F238" s="36" t="n">
         <v>5.05</v>
       </c>
-      <c r="G238" s="65" t="s"/>
-    </row>
-    <row customHeight="true" ht="22.5" outlineLevel="0" r="239">
-      <c r="A239" s="31" t="n"/>
-      <c r="B239" s="32" t="n">
+      <c r="G238" s="66" t="s"/>
+    </row>
+    <row customHeight="true" ht="36.2412109375" outlineLevel="0" r="239">
+      <c r="A239" s="33" t="n">
+        <v>228</v>
+      </c>
+      <c r="B239" s="31" t="n"/>
+      <c r="C239" s="67" t="s">
+        <v>244</v>
+      </c>
+      <c r="D239" s="68" t="s"/>
+      <c r="E239" s="69" t="s"/>
+      <c r="F239" s="70" t="s"/>
+      <c r="G239" s="71" t="s"/>
+    </row>
+    <row customHeight="true" ht="22.5" outlineLevel="0" r="240">
+      <c r="A240" s="34" t="n"/>
+      <c r="B240" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="C239" s="33" t="s">
+      <c r="C240" s="32" t="s">
         <v>245</v>
       </c>
-      <c r="D239" s="66" t="s">
+      <c r="D240" s="72" t="s"/>
+      <c r="E240" s="73" t="s"/>
+      <c r="F240" s="74" t="s"/>
+      <c r="G240" s="75" t="s"/>
+    </row>
+    <row ht="0" outlineLevel="0" r="241">
+      <c r="A241" s="33" t="n">
+        <v>229</v>
+      </c>
+      <c r="B241" s="44" t="n"/>
+      <c r="C241" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="E239" s="67" t="s"/>
-      <c r="F239" s="57" t="s">
-        <v>242</v>
-      </c>
-      <c r="G239" s="68" t="s"/>
-    </row>
-    <row customHeight="true" ht="52.25" outlineLevel="0" r="240">
-      <c r="A240" s="34" t="n">
-        <v>228</v>
-      </c>
-      <c r="B240" s="43" t="n"/>
-      <c r="C240" s="30" t="s">
-        <v>247</v>
-      </c>
-      <c r="D240" s="69" t="s"/>
-      <c r="E240" s="70" t="s"/>
-      <c r="F240" s="71" t="s"/>
-      <c r="G240" s="72" t="s"/>
-    </row>
-    <row customHeight="true" ht="35.25" outlineLevel="0" r="241">
-      <c r="A241" s="37" t="n">
-        <v>229</v>
-      </c>
-      <c r="B241" s="31" t="n"/>
-      <c r="C241" s="30" t="s">
-        <v>248</v>
-      </c>
-      <c r="D241" s="73" t="s"/>
-      <c r="E241" s="74" t="s"/>
-      <c r="F241" s="39" t="n">
-        <v>9.65</v>
-      </c>
-      <c r="G241" s="75" t="s"/>
-    </row>
-    <row customHeight="true" ht="36.75" outlineLevel="0" r="242">
-      <c r="A242" s="37" t="n">
-        <v>230</v>
-      </c>
-      <c r="B242" s="31" t="n"/>
-      <c r="C242" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="D242" s="76" t="s"/>
-      <c r="E242" s="77" t="s"/>
-      <c r="F242" s="78" t="s"/>
-      <c r="G242" s="79" t="s"/>
-    </row>
-    <row customHeight="true" ht="13.5" outlineLevel="0" r="243">
-      <c r="A243" s="35" t="n"/>
-      <c r="B243" s="32" t="n">
-        <v>4</v>
-      </c>
-      <c r="C243" s="33" t="s">
-        <v>250</v>
-      </c>
-      <c r="D243" s="80" t="s"/>
-      <c r="E243" s="81" t="s"/>
-      <c r="F243" s="82" t="s"/>
-      <c r="G243" s="83" t="s"/>
-    </row>
-    <row customHeight="true" ht="49.25" outlineLevel="0" r="244">
-      <c r="A244" s="34" t="n">
-        <v>231</v>
-      </c>
-      <c r="B244" s="43" t="n"/>
-      <c r="C244" s="38" t="s">
-        <v>251</v>
-      </c>
-      <c r="D244" s="84" t="s"/>
-      <c r="E244" s="85" t="s"/>
-      <c r="F244" s="86" t="s"/>
-      <c r="G244" s="87" t="s"/>
-    </row>
+      <c r="D241" s="76" t="s"/>
+      <c r="E241" s="77" t="s"/>
+      <c r="F241" s="78" t="s"/>
+      <c r="G241" s="79" t="s"/>
+    </row>
+    <row customHeight="true" ht="35.25" outlineLevel="0" r="242"/>
+    <row customHeight="true" ht="36.75" outlineLevel="0" r="243"/>
+    <row customHeight="true" ht="13.5" outlineLevel="0" r="244"/>
+    <row customHeight="true" ht="49.25" outlineLevel="0" r="245"/>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="23">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:G3"/>
@@ -8425,27 +8265,22 @@
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
     <mergeCell ref="D7:G7"/>
-    <mergeCell ref="C7:C9"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="C244:G244"/>
-    <mergeCell ref="C243:G243"/>
-    <mergeCell ref="C242:G242"/>
-    <mergeCell ref="F241:G241"/>
-    <mergeCell ref="C240:G240"/>
-    <mergeCell ref="F239:G239"/>
     <mergeCell ref="F238:G238"/>
     <mergeCell ref="C237:G237"/>
     <mergeCell ref="F236:G236"/>
     <mergeCell ref="C235:G235"/>
     <mergeCell ref="C234:G234"/>
     <mergeCell ref="C233:G233"/>
-    <mergeCell ref="C241:E241"/>
+    <mergeCell ref="C239:G239"/>
     <mergeCell ref="B197:C197"/>
-    <mergeCell ref="D239:E239"/>
     <mergeCell ref="C238:E238"/>
     <mergeCell ref="D236:E236"/>
+    <mergeCell ref="C241:G241"/>
+    <mergeCell ref="C240:G240"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.300000011920929" header="0.300000011920929" left="0.700000047683716" right="0.700000047683716" top="0.75"/>
 </worksheet>

</xml_diff>